<commit_message>
admin display-> pengguna,penyedia, produk, transaksi -> upload databse db_cashier-1
</commit_message>
<xml_diff>
--- a/myfile/Information.xlsx
+++ b/myfile/Information.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="23040" windowHeight="9204"/>
+    <workbookView windowWidth="23040" windowHeight="9204" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Rules" sheetId="2" r:id="rId1"/>
@@ -152,8 +152,95 @@
             <charset val="0"/>
           </rPr>
           <t xml:space="preserve">
-login level user
-harus finish</t>
+login level user finish</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="E8" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <rFont val="Times New Roman"/>
+            <charset val="0"/>
+          </rPr>
+          <t>user:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <rFont val="Times New Roman"/>
+            <charset val="0"/>
+          </rPr>
+          <t xml:space="preserve">
+Desain Mockup 5%</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="F8" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <rFont val="Times New Roman"/>
+            <charset val="0"/>
+          </rPr>
+          <t>user:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <rFont val="Times New Roman"/>
+            <charset val="0"/>
+          </rPr>
+          <t xml:space="preserve">
+konsultasi database sama kak azhar</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="G8" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <rFont val="Times New Roman"/>
+            <charset val="0"/>
+          </rPr>
+          <t>user:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <rFont val="Times New Roman"/>
+            <charset val="0"/>
+          </rPr>
+          <t xml:space="preserve">
+display data admin 5%</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="I8" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <rFont val="Times New Roman"/>
+            <charset val="0"/>
+          </rPr>
+          <t>user:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <rFont val="Times New Roman"/>
+            <charset val="0"/>
+          </rPr>
+          <t xml:space="preserve">
+display admin 10%</t>
         </r>
       </text>
     </comment>
@@ -184,7 +271,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="58">
   <si>
     <t>Rules</t>
   </si>
@@ -346,6 +433,18 @@
   </si>
   <si>
     <t>Saturday</t>
+  </si>
+  <si>
+    <t>Coding</t>
+  </si>
+  <si>
+    <t>Design</t>
+  </si>
+  <si>
+    <t>Nganggur</t>
+  </si>
+  <si>
+    <t>Lainnya</t>
   </si>
 </sst>
 </file>
@@ -404,6 +503,13 @@
     </font>
     <font>
       <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
@@ -411,7 +517,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF006100"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -433,47 +539,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -487,10 +553,11 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF006100"/>
+      <color theme="3"/>
       <name val="Calibri"/>
-      <charset val="0"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -512,7 +579,23 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -526,8 +609,24 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF9C6500"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -541,7 +640,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -558,7 +657,7 @@
       <charset val="0"/>
     </font>
   </fonts>
-  <fills count="33">
+  <fills count="37">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -567,49 +666,193 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFFFC7CE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="4" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="6" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -621,25 +864,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
+        <fgColor theme="6" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -649,110 +874,8 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="49">
+  <borders count="51">
     <border>
       <left/>
       <right/>
@@ -784,7 +907,9 @@
       <left style="medium">
         <color auto="1"/>
       </left>
-      <right/>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
       <top style="medium">
         <color auto="1"/>
       </top>
@@ -794,18 +919,216 @@
       <diagonal/>
     </border>
     <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left/>
       <right/>
+      <top/>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
       <top style="medium">
         <color auto="1"/>
       </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top/>
       <bottom style="medium">
         <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
-      <left style="medium">
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="dashed">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top style="dashed">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="dashed">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="dashed">
         <color auto="1"/>
       </left>
       <right/>
@@ -817,171 +1140,6 @@
       <left style="medium">
         <color auto="1"/>
       </left>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="medium">
-        <color auto="1"/>
-      </right>
-      <top style="medium">
-        <color auto="1"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="medium">
-        <color auto="1"/>
-      </right>
-      <top style="medium">
-        <color auto="1"/>
-      </top>
-      <bottom style="medium">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="medium">
-        <color auto="1"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="medium">
-        <color auto="1"/>
-      </right>
-      <top/>
-      <bottom style="medium">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="dashed">
-        <color auto="1"/>
-      </left>
-      <right/>
-      <top style="dashed">
-        <color auto="1"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="dashed">
-        <color auto="1"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="dashed">
-        <color auto="1"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color auto="1"/>
-      </left>
       <right style="thin">
         <color auto="1"/>
       </right>
@@ -1017,19 +1175,6 @@
         <color auto="1"/>
       </top>
       <bottom style="medium">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color auto="1"/>
-      </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top/>
-      <bottom style="thin">
         <color auto="1"/>
       </bottom>
       <diagonal/>
@@ -1055,21 +1200,6 @@
       <top style="thin">
         <color auto="1"/>
       </top>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color auto="1"/>
-      </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
       <bottom/>
       <diagonal/>
     </border>
@@ -1123,7 +1253,7 @@
       <top style="medium">
         <color auto="1"/>
       </top>
-      <bottom style="medium">
+      <bottom style="thin">
         <color auto="1"/>
       </bottom>
       <diagonal/>
@@ -1135,7 +1265,7 @@
       <right style="medium">
         <color auto="1"/>
       </right>
-      <top style="medium">
+      <top style="thin">
         <color auto="1"/>
       </top>
       <bottom style="thin">
@@ -1153,21 +1283,6 @@
       <top style="thin">
         <color auto="1"/>
       </top>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color auto="1"/>
-      </left>
-      <right style="medium">
-        <color auto="1"/>
-      </right>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
       <bottom/>
       <diagonal/>
     </border>
@@ -1186,7 +1301,53 @@
       <left style="medium">
         <color auto="1"/>
       </left>
+      <right/>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
       <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
         <color auto="1"/>
       </right>
       <top/>
@@ -1232,36 +1393,6 @@
       <top/>
       <bottom style="medium">
         <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1286,6 +1417,60 @@
       <diagonal/>
     </border>
     <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin">
         <color rgb="FF3F3F3F"/>
       </left>
@@ -1300,36 +1485,12 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -1347,134 +1508,134 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="6" borderId="42" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="41" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="47" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="14" borderId="46" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="43" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="21" borderId="47" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="43" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="45" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="32" borderId="48" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="23" borderId="50" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="23" borderId="48" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="49" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="44" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="41" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="45" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="19" borderId="43" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="8" borderId="46" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="8" borderId="43" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="48" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="44" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="68">
+  <cellXfs count="79">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1490,202 +1651,235 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="6" xfId="0" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="7" xfId="0" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="12" xfId="0" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="13" xfId="0" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="39" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="40" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="41" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="35" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="36" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="38" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="39" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1" quotePrefix="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="39" xfId="0" applyBorder="1" applyAlignment="1" quotePrefix="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1" quotePrefix="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1" applyAlignment="1" quotePrefix="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1" quotePrefix="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -2009,202 +2203,202 @@
   <sheetPr/>
   <dimension ref="C4:F20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I8" sqref="I8:J13"/>
+    <sheetView topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="16" customHeight="1" outlineLevelCol="5"/>
   <cols>
-    <col min="1" max="3" width="8.88888888888889" style="18"/>
-    <col min="4" max="4" width="3.44444444444444" style="18" customWidth="1"/>
-    <col min="5" max="5" width="31.6666666666667" style="18" customWidth="1"/>
-    <col min="6" max="6" width="21" style="18" customWidth="1"/>
-    <col min="7" max="16384" width="8.88888888888889" style="18"/>
+    <col min="1" max="3" width="8.88888888888889" style="29"/>
+    <col min="4" max="4" width="3.44444444444444" style="29" customWidth="1"/>
+    <col min="5" max="5" width="31.6666666666667" style="29" customWidth="1"/>
+    <col min="6" max="6" width="21" style="29" customWidth="1"/>
+    <col min="7" max="16384" width="8.88888888888889" style="29"/>
   </cols>
   <sheetData>
     <row r="4" customHeight="1" spans="3:4">
-      <c r="C4" s="53"/>
-      <c r="D4" s="53"/>
+      <c r="C4" s="64"/>
+      <c r="D4" s="64"/>
     </row>
     <row r="5" customHeight="1" spans="3:6">
-      <c r="C5" s="54" t="s">
+      <c r="C5" s="65" t="s">
         <v>0</v>
       </c>
-      <c r="D5" s="55"/>
-      <c r="E5" s="55"/>
-      <c r="F5" s="56"/>
+      <c r="D5" s="66"/>
+      <c r="E5" s="66"/>
+      <c r="F5" s="67"/>
     </row>
     <row r="6" customHeight="1" spans="3:6">
-      <c r="C6" s="57" t="s">
+      <c r="C6" s="68" t="s">
         <v>1</v>
       </c>
-      <c r="D6" s="58">
+      <c r="D6" s="69">
         <v>1</v>
       </c>
-      <c r="E6" s="59" t="s">
+      <c r="E6" s="70" t="s">
         <v>2</v>
       </c>
-      <c r="F6" s="68" t="s">
+      <c r="F6" s="79" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="7" customHeight="1" spans="3:6">
-      <c r="C7" s="57"/>
-      <c r="D7" s="58">
+      <c r="C7" s="68"/>
+      <c r="D7" s="69">
         <v>2</v>
       </c>
-      <c r="E7" s="59" t="s">
+      <c r="E7" s="70" t="s">
         <v>4</v>
       </c>
-      <c r="F7" s="68" t="s">
+      <c r="F7" s="79" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="8" customHeight="1" spans="3:6">
-      <c r="C8" s="57"/>
-      <c r="D8" s="58">
+      <c r="C8" s="68"/>
+      <c r="D8" s="69">
         <v>3</v>
       </c>
-      <c r="E8" s="59" t="s">
+      <c r="E8" s="70" t="s">
         <v>6</v>
       </c>
-      <c r="F8" s="68" t="s">
+      <c r="F8" s="79" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="9" customHeight="1" spans="3:6">
-      <c r="C9" s="57"/>
-      <c r="D9" s="58">
+      <c r="C9" s="68"/>
+      <c r="D9" s="69">
         <v>4</v>
       </c>
-      <c r="E9" s="59" t="s">
+      <c r="E9" s="70" t="s">
         <v>7</v>
       </c>
-      <c r="F9" s="60"/>
+      <c r="F9" s="71"/>
     </row>
     <row r="10" customHeight="1" spans="3:6">
-      <c r="C10" s="57"/>
-      <c r="D10" s="58">
+      <c r="C10" s="68"/>
+      <c r="D10" s="69">
         <v>5</v>
       </c>
-      <c r="E10" s="59" t="s">
+      <c r="E10" s="70" t="s">
         <v>8</v>
       </c>
-      <c r="F10" s="60"/>
+      <c r="F10" s="71"/>
     </row>
     <row r="11" customHeight="1" spans="3:6">
-      <c r="C11" s="61"/>
-      <c r="D11" s="62">
+      <c r="C11" s="72"/>
+      <c r="D11" s="73">
         <v>6</v>
       </c>
-      <c r="E11" s="63" t="s">
+      <c r="E11" s="74" t="s">
         <v>9</v>
       </c>
-      <c r="F11" s="64"/>
+      <c r="F11" s="75"/>
     </row>
     <row r="12" customHeight="1" spans="3:6">
-      <c r="C12" s="57" t="s">
+      <c r="C12" s="68" t="s">
         <v>10</v>
       </c>
-      <c r="D12" s="59">
+      <c r="D12" s="70">
         <v>1</v>
       </c>
-      <c r="E12" s="59" t="s">
+      <c r="E12" s="70" t="s">
         <v>11</v>
       </c>
-      <c r="F12" s="68" t="s">
+      <c r="F12" s="79" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="13" customHeight="1" spans="3:6">
-      <c r="C13" s="57"/>
-      <c r="D13" s="59">
+      <c r="C13" s="68"/>
+      <c r="D13" s="70">
         <v>2</v>
       </c>
-      <c r="E13" s="59" t="s">
+      <c r="E13" s="70" t="s">
         <v>13</v>
       </c>
-      <c r="F13" s="68" t="s">
+      <c r="F13" s="79" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="14" customHeight="1" spans="3:6">
-      <c r="C14" s="57"/>
-      <c r="D14" s="59">
+      <c r="C14" s="68"/>
+      <c r="D14" s="70">
         <v>3</v>
       </c>
-      <c r="E14" s="59" t="s">
+      <c r="E14" s="70" t="s">
         <v>14</v>
       </c>
-      <c r="F14" s="68" t="s">
+      <c r="F14" s="79" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="15" customHeight="1" spans="3:6">
-      <c r="C15" s="57"/>
-      <c r="D15" s="59">
+      <c r="C15" s="68"/>
+      <c r="D15" s="70">
         <v>4</v>
       </c>
-      <c r="E15" s="59" t="s">
+      <c r="E15" s="70" t="s">
         <v>15</v>
       </c>
-      <c r="F15" s="68" t="s">
+      <c r="F15" s="79" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="16" customHeight="1" spans="3:6">
-      <c r="C16" s="57"/>
-      <c r="D16" s="59">
+      <c r="C16" s="68"/>
+      <c r="D16" s="70">
         <v>5</v>
       </c>
-      <c r="E16" s="59" t="s">
+      <c r="E16" s="70" t="s">
         <v>17</v>
       </c>
-      <c r="F16" s="68" t="s">
+      <c r="F16" s="79" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="17" customHeight="1" spans="3:6">
-      <c r="C17" s="57"/>
-      <c r="D17" s="59">
+      <c r="C17" s="68"/>
+      <c r="D17" s="70">
         <v>6</v>
       </c>
-      <c r="E17" s="59" t="s">
+      <c r="E17" s="70" t="s">
         <v>18</v>
       </c>
-      <c r="F17" s="68" t="s">
+      <c r="F17" s="79" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="18" customHeight="1" spans="3:6">
-      <c r="C18" s="57"/>
-      <c r="D18" s="59">
+      <c r="C18" s="68"/>
+      <c r="D18" s="70">
         <v>7</v>
       </c>
-      <c r="E18" s="59" t="s">
+      <c r="E18" s="70" t="s">
         <v>7</v>
       </c>
-      <c r="F18" s="60"/>
+      <c r="F18" s="71"/>
     </row>
     <row r="19" customHeight="1" spans="3:6">
-      <c r="C19" s="57"/>
-      <c r="D19" s="59">
+      <c r="C19" s="68"/>
+      <c r="D19" s="70">
         <v>8</v>
       </c>
-      <c r="E19" s="53" t="s">
+      <c r="E19" s="64" t="s">
         <v>8</v>
       </c>
-      <c r="F19" s="60"/>
+      <c r="F19" s="71"/>
     </row>
     <row r="20" customHeight="1" spans="3:6">
-      <c r="C20" s="65"/>
-      <c r="D20" s="66">
+      <c r="C20" s="76"/>
+      <c r="D20" s="77">
         <v>9</v>
       </c>
-      <c r="E20" s="66" t="s">
+      <c r="E20" s="77" t="s">
         <v>9</v>
       </c>
-      <c r="F20" s="67"/>
+      <c r="F20" s="78"/>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -2228,291 +2422,291 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="8.55555555555556" style="18" customWidth="1"/>
-    <col min="2" max="2" width="3.88888888888889" style="28" customWidth="1"/>
-    <col min="3" max="3" width="3.44444444444444" style="18" customWidth="1"/>
-    <col min="4" max="4" width="6.77777777777778" style="18" customWidth="1"/>
-    <col min="5" max="5" width="12.3333333333333" style="18" customWidth="1"/>
-    <col min="6" max="6" width="8.44444444444444" style="18" customWidth="1"/>
-    <col min="7" max="7" width="9.33333333333333" style="28" customWidth="1"/>
-    <col min="8" max="8" width="6.66666666666667" style="18" customWidth="1"/>
-    <col min="9" max="9" width="8.88888888888889" style="18"/>
-    <col min="10" max="10" width="3.22222222222222" style="18" customWidth="1"/>
-    <col min="11" max="16384" width="8.88888888888889" style="18"/>
+    <col min="1" max="1" width="8.55555555555556" style="29" customWidth="1"/>
+    <col min="2" max="2" width="3.88888888888889" style="39" customWidth="1"/>
+    <col min="3" max="3" width="3.44444444444444" style="29" customWidth="1"/>
+    <col min="4" max="4" width="6.77777777777778" style="29" customWidth="1"/>
+    <col min="5" max="5" width="12.3333333333333" style="29" customWidth="1"/>
+    <col min="6" max="6" width="8.44444444444444" style="29" customWidth="1"/>
+    <col min="7" max="7" width="9.33333333333333" style="39" customWidth="1"/>
+    <col min="8" max="8" width="6.66666666666667" style="29" customWidth="1"/>
+    <col min="9" max="9" width="8.88888888888889" style="29"/>
+    <col min="10" max="10" width="3.22222222222222" style="29" customWidth="1"/>
+    <col min="11" max="16384" width="8.88888888888889" style="29"/>
   </cols>
   <sheetData>
     <row r="3" spans="2:10">
-      <c r="B3" s="29"/>
-      <c r="C3" s="30"/>
-      <c r="D3" s="30"/>
-      <c r="E3" s="30"/>
-      <c r="F3" s="30"/>
-      <c r="G3" s="31"/>
-      <c r="H3" s="30"/>
-      <c r="I3" s="30"/>
-      <c r="J3" s="46"/>
+      <c r="B3" s="40"/>
+      <c r="C3" s="41"/>
+      <c r="D3" s="41"/>
+      <c r="E3" s="41"/>
+      <c r="F3" s="41"/>
+      <c r="G3" s="42"/>
+      <c r="H3" s="41"/>
+      <c r="I3" s="41"/>
+      <c r="J3" s="57"/>
     </row>
     <row r="4" ht="19" customHeight="1" spans="2:10">
-      <c r="B4" s="32"/>
-      <c r="C4" s="33" t="s">
+      <c r="B4" s="43"/>
+      <c r="C4" s="44" t="s">
         <v>19</v>
       </c>
-      <c r="D4" s="33"/>
-      <c r="E4" s="33"/>
-      <c r="F4" s="33"/>
-      <c r="G4" s="33"/>
-      <c r="H4" s="33"/>
-      <c r="I4" s="33"/>
-      <c r="J4" s="47"/>
+      <c r="D4" s="44"/>
+      <c r="E4" s="44"/>
+      <c r="F4" s="44"/>
+      <c r="G4" s="44"/>
+      <c r="H4" s="44"/>
+      <c r="I4" s="44"/>
+      <c r="J4" s="58"/>
     </row>
     <row r="5" ht="18" customHeight="1" spans="2:10">
-      <c r="B5" s="32"/>
-      <c r="C5" s="28"/>
-      <c r="G5" s="28" t="s">
+      <c r="B5" s="43"/>
+      <c r="C5" s="39"/>
+      <c r="G5" s="39" t="s">
         <v>20</v>
       </c>
-      <c r="H5" s="28"/>
-      <c r="I5" s="28"/>
-      <c r="J5" s="47"/>
+      <c r="H5" s="39"/>
+      <c r="I5" s="39"/>
+      <c r="J5" s="58"/>
     </row>
     <row r="6" ht="16" customHeight="1" spans="2:10">
-      <c r="B6" s="32"/>
-      <c r="C6" s="28"/>
-      <c r="G6" s="18"/>
-      <c r="H6" s="28"/>
-      <c r="J6" s="47"/>
+      <c r="B6" s="43"/>
+      <c r="C6" s="39"/>
+      <c r="G6" s="29"/>
+      <c r="H6" s="39"/>
+      <c r="J6" s="58"/>
     </row>
     <row r="7" ht="15.15" spans="2:10">
-      <c r="B7" s="32"/>
-      <c r="C7" s="28"/>
-      <c r="D7" s="34" t="s">
+      <c r="B7" s="43"/>
+      <c r="C7" s="39"/>
+      <c r="D7" s="45" t="s">
         <v>21</v>
       </c>
-      <c r="E7" s="34"/>
-      <c r="F7" s="34"/>
-      <c r="G7" s="34"/>
-      <c r="H7" s="28"/>
-      <c r="I7" s="34"/>
-      <c r="J7" s="47"/>
+      <c r="E7" s="45"/>
+      <c r="F7" s="45"/>
+      <c r="G7" s="45"/>
+      <c r="H7" s="39"/>
+      <c r="I7" s="45"/>
+      <c r="J7" s="58"/>
     </row>
     <row r="8" ht="29.55" spans="2:10">
-      <c r="B8" s="32"/>
-      <c r="C8" s="35" t="s">
+      <c r="B8" s="43"/>
+      <c r="C8" s="46" t="s">
         <v>22</v>
       </c>
-      <c r="D8" s="36" t="s">
+      <c r="D8" s="47" t="s">
         <v>23</v>
       </c>
-      <c r="E8" s="36" t="s">
+      <c r="E8" s="47" t="s">
         <v>24</v>
       </c>
-      <c r="F8" s="36" t="s">
+      <c r="F8" s="47" t="s">
         <v>25</v>
       </c>
-      <c r="G8" s="36" t="s">
+      <c r="G8" s="47" t="s">
         <v>26</v>
       </c>
-      <c r="H8" s="37" t="s">
+      <c r="H8" s="48" t="s">
         <v>27</v>
       </c>
-      <c r="I8" s="48" t="s">
+      <c r="I8" s="59" t="s">
         <v>28</v>
       </c>
-      <c r="J8" s="47"/>
+      <c r="J8" s="58"/>
     </row>
     <row r="9" spans="2:10">
-      <c r="B9" s="32"/>
-      <c r="C9" s="38">
+      <c r="B9" s="43"/>
+      <c r="C9" s="49">
         <v>1</v>
       </c>
-      <c r="D9" s="26"/>
-      <c r="E9" s="26"/>
-      <c r="F9" s="26"/>
-      <c r="G9" s="26"/>
-      <c r="H9" s="69" t="s">
+      <c r="D9" s="37"/>
+      <c r="E9" s="37"/>
+      <c r="F9" s="37"/>
+      <c r="G9" s="37"/>
+      <c r="H9" s="80" t="s">
         <v>29</v>
       </c>
-      <c r="I9" s="49"/>
-      <c r="J9" s="47"/>
+      <c r="I9" s="60"/>
+      <c r="J9" s="58"/>
     </row>
     <row r="10" spans="2:10">
-      <c r="B10" s="32"/>
-      <c r="C10" s="40">
+      <c r="B10" s="43"/>
+      <c r="C10" s="51">
         <v>2</v>
       </c>
-      <c r="D10" s="41"/>
-      <c r="E10" s="41"/>
-      <c r="F10" s="41"/>
-      <c r="G10" s="41"/>
-      <c r="H10" s="69" t="s">
+      <c r="D10" s="52"/>
+      <c r="E10" s="52"/>
+      <c r="F10" s="52"/>
+      <c r="G10" s="52"/>
+      <c r="H10" s="80" t="s">
         <v>29</v>
       </c>
-      <c r="I10" s="50"/>
-      <c r="J10" s="47"/>
+      <c r="I10" s="61"/>
+      <c r="J10" s="58"/>
     </row>
     <row r="11" spans="2:10">
-      <c r="B11" s="32"/>
-      <c r="C11" s="40">
+      <c r="B11" s="43"/>
+      <c r="C11" s="51">
         <v>3</v>
       </c>
-      <c r="D11" s="41"/>
-      <c r="E11" s="41"/>
-      <c r="F11" s="41"/>
-      <c r="G11" s="41"/>
-      <c r="H11" s="69" t="s">
+      <c r="D11" s="52"/>
+      <c r="E11" s="52"/>
+      <c r="F11" s="52"/>
+      <c r="G11" s="52"/>
+      <c r="H11" s="80" t="s">
         <v>29</v>
       </c>
-      <c r="I11" s="50"/>
-      <c r="J11" s="47"/>
+      <c r="I11" s="61"/>
+      <c r="J11" s="58"/>
     </row>
     <row r="12" spans="2:10">
-      <c r="B12" s="32"/>
-      <c r="C12" s="40">
+      <c r="B12" s="43"/>
+      <c r="C12" s="51">
         <v>4</v>
       </c>
-      <c r="D12" s="41"/>
-      <c r="E12" s="41"/>
-      <c r="F12" s="41"/>
-      <c r="G12" s="41"/>
-      <c r="H12" s="69" t="s">
+      <c r="D12" s="52"/>
+      <c r="E12" s="52"/>
+      <c r="F12" s="52"/>
+      <c r="G12" s="52"/>
+      <c r="H12" s="80" t="s">
         <v>29</v>
       </c>
-      <c r="I12" s="50"/>
-      <c r="J12" s="47"/>
+      <c r="I12" s="61"/>
+      <c r="J12" s="58"/>
     </row>
     <row r="13" spans="2:10">
-      <c r="B13" s="32"/>
-      <c r="C13" s="40">
+      <c r="B13" s="43"/>
+      <c r="C13" s="51">
         <v>5</v>
       </c>
-      <c r="D13" s="41"/>
-      <c r="E13" s="41"/>
-      <c r="F13" s="41"/>
-      <c r="G13" s="41"/>
-      <c r="H13" s="69" t="s">
+      <c r="D13" s="52"/>
+      <c r="E13" s="52"/>
+      <c r="F13" s="52"/>
+      <c r="G13" s="52"/>
+      <c r="H13" s="80" t="s">
         <v>29</v>
       </c>
-      <c r="I13" s="50"/>
-      <c r="J13" s="47"/>
+      <c r="I13" s="61"/>
+      <c r="J13" s="58"/>
     </row>
     <row r="14" spans="2:10">
-      <c r="B14" s="32"/>
-      <c r="C14" s="40">
+      <c r="B14" s="43"/>
+      <c r="C14" s="51">
         <v>6</v>
       </c>
-      <c r="D14" s="41"/>
-      <c r="E14" s="41"/>
-      <c r="F14" s="41"/>
-      <c r="G14" s="41"/>
-      <c r="H14" s="69" t="s">
+      <c r="D14" s="52"/>
+      <c r="E14" s="52"/>
+      <c r="F14" s="52"/>
+      <c r="G14" s="52"/>
+      <c r="H14" s="80" t="s">
         <v>29</v>
       </c>
-      <c r="I14" s="50"/>
-      <c r="J14" s="47"/>
+      <c r="I14" s="61"/>
+      <c r="J14" s="58"/>
     </row>
     <row r="15" ht="15.15" spans="2:10">
-      <c r="B15" s="32"/>
-      <c r="C15" s="42"/>
-      <c r="D15" s="22"/>
-      <c r="E15" s="22"/>
-      <c r="F15" s="22"/>
-      <c r="G15" s="22"/>
-      <c r="H15" s="69" t="s">
+      <c r="B15" s="43"/>
+      <c r="C15" s="53"/>
+      <c r="D15" s="33"/>
+      <c r="E15" s="33"/>
+      <c r="F15" s="33"/>
+      <c r="G15" s="33"/>
+      <c r="H15" s="80" t="s">
         <v>29</v>
       </c>
-      <c r="I15" s="51"/>
-      <c r="J15" s="47"/>
+      <c r="I15" s="62"/>
+      <c r="J15" s="58"/>
     </row>
     <row r="16" ht="15.15" spans="2:10">
-      <c r="B16" s="32"/>
-      <c r="C16" s="35" t="s">
+      <c r="B16" s="43"/>
+      <c r="C16" s="46" t="s">
         <v>30</v>
       </c>
-      <c r="D16" s="36"/>
-      <c r="E16" s="36"/>
-      <c r="F16" s="36"/>
-      <c r="G16" s="36"/>
-      <c r="H16" s="37"/>
-      <c r="I16" s="70" t="s">
+      <c r="D16" s="47"/>
+      <c r="E16" s="47"/>
+      <c r="F16" s="47"/>
+      <c r="G16" s="47"/>
+      <c r="H16" s="48"/>
+      <c r="I16" s="81" t="s">
         <v>29</v>
       </c>
-      <c r="J16" s="47"/>
+      <c r="J16" s="58"/>
     </row>
     <row r="17" spans="2:10">
-      <c r="B17" s="43"/>
-      <c r="C17" s="44"/>
-      <c r="D17" s="44"/>
-      <c r="E17" s="44"/>
-      <c r="F17" s="44"/>
-      <c r="G17" s="45"/>
-      <c r="H17" s="44"/>
-      <c r="I17" s="44"/>
-      <c r="J17" s="52"/>
+      <c r="B17" s="54"/>
+      <c r="C17" s="55"/>
+      <c r="D17" s="55"/>
+      <c r="E17" s="55"/>
+      <c r="F17" s="55"/>
+      <c r="G17" s="56"/>
+      <c r="H17" s="55"/>
+      <c r="I17" s="55"/>
+      <c r="J17" s="63"/>
     </row>
     <row r="18" ht="17" customHeight="1"/>
     <row r="19" ht="13" customHeight="1" spans="12:13">
-      <c r="L19" s="18">
+      <c r="L19" s="29">
         <v>1</v>
       </c>
-      <c r="M19" s="18">
+      <c r="M19" s="29">
         <v>2</v>
       </c>
     </row>
     <row r="20" spans="12:15">
-      <c r="L20" s="18">
+      <c r="L20" s="29">
         <v>2</v>
       </c>
-      <c r="M20" s="18">
+      <c r="M20" s="29">
         <v>3</v>
       </c>
-      <c r="N20" s="18">
+      <c r="N20" s="29">
         <v>4</v>
       </c>
-      <c r="O20" s="18">
+      <c r="O20" s="29">
         <v>5</v>
       </c>
     </row>
     <row r="21" spans="13:15">
-      <c r="M21" s="18">
+      <c r="M21" s="29">
         <v>4</v>
       </c>
-      <c r="O21" s="18">
+      <c r="O21" s="29">
         <v>6</v>
       </c>
     </row>
     <row r="22" spans="13:15">
-      <c r="M22" s="18">
+      <c r="M22" s="29">
         <v>5</v>
       </c>
-      <c r="N22" s="18">
+      <c r="N22" s="29">
         <v>6</v>
       </c>
-      <c r="O22" s="18">
+      <c r="O22" s="29">
         <v>7</v>
       </c>
     </row>
     <row r="23" spans="14:14">
-      <c r="N23" s="18">
+      <c r="N23" s="29">
         <v>8</v>
       </c>
     </row>
     <row r="25" spans="14:14">
-      <c r="N25" s="18">
+      <c r="N25" s="29">
         <v>10</v>
       </c>
     </row>
     <row r="26" spans="14:14">
-      <c r="N26" s="18">
+      <c r="N26" s="29">
         <v>12</v>
       </c>
     </row>
     <row r="28" spans="14:14">
-      <c r="N28" s="18">
+      <c r="N28" s="29">
         <v>14</v>
       </c>
     </row>
     <row r="29" spans="14:14">
-      <c r="N29" s="18">
+      <c r="N29" s="29">
         <v>16</v>
       </c>
     </row>
@@ -2539,73 +2733,73 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="14.4" outlineLevelCol="4"/>
   <cols>
-    <col min="1" max="1" width="13.4444444444444" style="18" customWidth="1"/>
-    <col min="2" max="2" width="17.8888888888889" style="18" customWidth="1"/>
-    <col min="3" max="4" width="31" style="18" customWidth="1"/>
-    <col min="5" max="5" width="20.1944444444444" style="18" customWidth="1"/>
-    <col min="6" max="16384" width="8.88888888888889" style="18"/>
+    <col min="1" max="1" width="13.4444444444444" style="29" customWidth="1"/>
+    <col min="2" max="2" width="17.8888888888889" style="29" customWidth="1"/>
+    <col min="3" max="4" width="31" style="29" customWidth="1"/>
+    <col min="5" max="5" width="20.1944444444444" style="29" customWidth="1"/>
+    <col min="6" max="16384" width="8.88888888888889" style="29"/>
   </cols>
   <sheetData>
     <row r="5" ht="15.6" spans="2:4">
-      <c r="B5" s="19" t="s">
+      <c r="B5" s="30" t="s">
         <v>31</v>
       </c>
-      <c r="C5" s="19"/>
-      <c r="D5" s="19"/>
+      <c r="C5" s="30"/>
+      <c r="D5" s="30"/>
     </row>
     <row r="6" spans="2:5">
-      <c r="B6" s="20" t="s">
+      <c r="B6" s="31" t="s">
         <v>32</v>
       </c>
-      <c r="C6" s="20" t="s">
+      <c r="C6" s="31" t="s">
         <v>33</v>
       </c>
-      <c r="D6" s="20" t="s">
+      <c r="D6" s="31" t="s">
         <v>34</v>
       </c>
-      <c r="E6" s="21"/>
+      <c r="E6" s="32"/>
     </row>
     <row r="7" ht="16" customHeight="1" spans="2:4">
-      <c r="B7" s="22" t="s">
+      <c r="B7" s="33" t="s">
         <v>35</v>
       </c>
-      <c r="C7" s="23" t="s">
+      <c r="C7" s="34" t="s">
         <v>36</v>
       </c>
-      <c r="D7" s="23" t="s">
+      <c r="D7" s="34" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="8" ht="16" customHeight="1" spans="2:4">
-      <c r="B8" s="24" t="s">
+      <c r="B8" s="35" t="s">
         <v>38</v>
       </c>
-      <c r="C8" s="23" t="s">
+      <c r="C8" s="34" t="s">
         <v>39</v>
       </c>
-      <c r="D8" s="23" t="s">
+      <c r="D8" s="34" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="9" ht="16" customHeight="1" spans="2:4">
-      <c r="B9" s="25" t="s">
+      <c r="B9" s="36" t="s">
         <v>41</v>
       </c>
-      <c r="C9" s="23" t="s">
+      <c r="C9" s="34" t="s">
         <v>42</v>
       </c>
-      <c r="D9" s="23" t="s">
+      <c r="D9" s="34" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="10" ht="16" customHeight="1" spans="2:4">
-      <c r="B10" s="26" t="s">
+      <c r="B10" s="37" t="s">
         <v>44</v>
       </c>
-      <c r="C10" s="27" t="s">
+      <c r="C10" s="38" t="s">
         <v>42</v>
       </c>
-      <c r="D10" s="27" t="s">
+      <c r="D10" s="38" t="s">
         <v>45</v>
       </c>
     </row>
@@ -2621,10 +2815,10 @@
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="C4:I11"/>
+  <dimension ref="C4:K11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="P5" sqref="P5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="N7" sqref="N7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="14.4"/>
@@ -2642,143 +2836,155 @@
       <c r="F5" s="3"/>
       <c r="G5" s="3"/>
       <c r="H5" s="3"/>
-      <c r="I5" s="13"/>
+      <c r="I5" s="20"/>
     </row>
     <row r="6" s="1" customFormat="1" ht="18" customHeight="1" spans="3:9">
       <c r="C6" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="D6" s="5" t="s">
+      <c r="D6" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="E6" s="5" t="s">
+      <c r="E6" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="F6" s="5" t="s">
+      <c r="F6" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="G6" s="5" t="s">
+      <c r="G6" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="H6" s="5" t="s">
+      <c r="H6" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="I6" s="14" t="s">
+      <c r="I6" s="4" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="7" ht="52" customHeight="1" spans="3:9">
-      <c r="C7" s="6">
+    <row r="7" ht="52" customHeight="1" spans="3:11">
+      <c r="C7" s="5">
         <v>1</v>
       </c>
-      <c r="D7" s="7">
+      <c r="D7" s="6">
         <v>2</v>
       </c>
       <c r="E7" s="7">
         <v>3</v>
       </c>
-      <c r="F7" s="7">
+      <c r="F7" s="8">
         <v>4</v>
       </c>
-      <c r="G7" s="7">
+      <c r="G7" s="8">
         <v>5</v>
       </c>
-      <c r="H7" s="7">
+      <c r="H7" s="9">
         <v>6</v>
       </c>
-      <c r="I7" s="15">
+      <c r="I7" s="21">
         <v>7</v>
       </c>
-    </row>
-    <row r="8" ht="52" customHeight="1" spans="3:9">
-      <c r="C8" s="8">
+      <c r="K7" s="22" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="8" ht="52" customHeight="1" spans="3:11">
+      <c r="C8" s="10">
         <v>8</v>
       </c>
-      <c r="D8" s="9">
+      <c r="D8" s="11">
         <v>9</v>
       </c>
-      <c r="E8" s="9">
+      <c r="E8" s="12">
         <v>10</v>
       </c>
-      <c r="F8" s="9">
+      <c r="F8" s="13">
         <v>11</v>
       </c>
-      <c r="G8" s="9">
+      <c r="G8" s="14">
         <v>12</v>
       </c>
-      <c r="H8" s="9">
+      <c r="H8" s="11">
         <v>13</v>
       </c>
-      <c r="I8" s="16">
+      <c r="I8" s="23">
         <v>14</v>
       </c>
-    </row>
-    <row r="9" ht="52" customHeight="1" spans="3:9">
-      <c r="C9" s="8">
+      <c r="K8" s="24" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="9" ht="52" customHeight="1" spans="3:11">
+      <c r="C9" s="15">
         <v>15</v>
       </c>
-      <c r="D9" s="9">
+      <c r="D9" s="16">
         <v>16</v>
       </c>
-      <c r="E9" s="9">
+      <c r="E9" s="16">
         <v>17</v>
       </c>
-      <c r="F9" s="9">
+      <c r="F9" s="16">
         <v>18</v>
       </c>
-      <c r="G9" s="9">
+      <c r="G9" s="16">
         <v>19</v>
       </c>
-      <c r="H9" s="9">
+      <c r="H9" s="16">
         <v>20</v>
       </c>
-      <c r="I9" s="16">
+      <c r="I9" s="25">
         <v>21</v>
       </c>
-    </row>
-    <row r="10" ht="52" customHeight="1" spans="3:9">
-      <c r="C10" s="8">
+      <c r="K9" s="26" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="10" ht="52" customHeight="1" spans="3:11">
+      <c r="C10" s="15">
         <v>22</v>
       </c>
-      <c r="D10" s="9">
+      <c r="D10" s="16">
         <v>23</v>
       </c>
-      <c r="E10" s="9">
+      <c r="E10" s="16">
         <v>24</v>
       </c>
-      <c r="F10" s="9">
+      <c r="F10" s="16">
         <v>25</v>
       </c>
-      <c r="G10" s="9">
+      <c r="G10" s="16">
         <v>26</v>
       </c>
-      <c r="H10" s="9">
+      <c r="H10" s="16">
         <v>27</v>
       </c>
-      <c r="I10" s="16">
+      <c r="I10" s="25">
         <v>28</v>
       </c>
+      <c r="K10" s="27" t="s">
+        <v>57</v>
+      </c>
     </row>
     <row r="11" ht="52" customHeight="1" spans="3:9">
-      <c r="C11" s="10">
+      <c r="C11" s="17">
         <v>29</v>
       </c>
-      <c r="D11" s="11">
+      <c r="D11" s="18">
         <v>30</v>
       </c>
-      <c r="E11" s="12">
+      <c r="E11" s="19">
         <v>1</v>
       </c>
-      <c r="F11" s="12">
+      <c r="F11" s="19">
         <v>2</v>
       </c>
-      <c r="G11" s="12">
+      <c r="G11" s="19">
         <v>3</v>
       </c>
-      <c r="H11" s="12">
+      <c r="H11" s="19">
         <v>4</v>
       </c>
-      <c r="I11" s="17">
+      <c r="I11" s="28">
         <v>5</v>
       </c>
     </row>

</xml_diff>

<commit_message>
admin -> display edit tambah
</commit_message>
<xml_diff>
--- a/myfile/Information.xlsx
+++ b/myfile/Information.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="23040" windowHeight="9204" activeTab="3"/>
+    <workbookView windowWidth="23040" windowHeight="9204" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Rules" sheetId="2" r:id="rId1"/>
@@ -244,6 +244,28 @@
         </r>
       </text>
     </comment>
+    <comment ref="D9" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <rFont val="Times New Roman"/>
+            <charset val="0"/>
+          </rPr>
+          <t>user:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <rFont val="Times New Roman"/>
+            <charset val="0"/>
+          </rPr>
+          <t xml:space="preserve">
+display admin 50%</t>
+        </r>
+      </text>
+    </comment>
     <comment ref="D11" authorId="0">
       <text>
         <r>
@@ -453,9 +475,9 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
     <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
   <fonts count="27">
     <font>
@@ -503,21 +525,21 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="0"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C0006"/>
+      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF006100"/>
+      <color theme="0"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -531,25 +553,18 @@
     </font>
     <font>
       <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
-      <sz val="11"/>
-      <color theme="1"/>
+      <sz val="13"/>
+      <color theme="3"/>
       <name val="Calibri"/>
-      <charset val="0"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -558,6 +573,29 @@
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -579,23 +617,7 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
+      <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -611,7 +633,14 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -626,21 +655,14 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
+      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -690,187 +712,187 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1384,6 +1406,21 @@
       <top/>
       <bottom style="medium">
         <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1393,6 +1430,60 @@
       <top/>
       <bottom style="medium">
         <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1411,77 +1502,8 @@
       <left/>
       <right/>
       <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
       <bottom style="double">
         <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1490,7 +1512,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -1508,134 +1530,134 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="14" borderId="46" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="43" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="21" borderId="47" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="9" borderId="43" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="44" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="22" borderId="48" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="44" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="46" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="16" borderId="45" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="20" borderId="47" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="20" borderId="45" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="50" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="49" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="43" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="45" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="32" borderId="48" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="23" borderId="50" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="23" borderId="48" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="49" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="44" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
   </cellStyleXfs>
-  <cellXfs count="79">
+  <cellXfs count="80">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1681,10 +1703,13 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1">
@@ -2209,196 +2234,196 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="16" customHeight="1" outlineLevelCol="5"/>
   <cols>
-    <col min="1" max="3" width="8.88888888888889" style="29"/>
-    <col min="4" max="4" width="3.44444444444444" style="29" customWidth="1"/>
-    <col min="5" max="5" width="31.6666666666667" style="29" customWidth="1"/>
-    <col min="6" max="6" width="21" style="29" customWidth="1"/>
-    <col min="7" max="16384" width="8.88888888888889" style="29"/>
+    <col min="1" max="3" width="8.88888888888889" style="30"/>
+    <col min="4" max="4" width="3.44444444444444" style="30" customWidth="1"/>
+    <col min="5" max="5" width="31.6666666666667" style="30" customWidth="1"/>
+    <col min="6" max="6" width="21" style="30" customWidth="1"/>
+    <col min="7" max="16384" width="8.88888888888889" style="30"/>
   </cols>
   <sheetData>
     <row r="4" customHeight="1" spans="3:4">
-      <c r="C4" s="64"/>
-      <c r="D4" s="64"/>
+      <c r="C4" s="65"/>
+      <c r="D4" s="65"/>
     </row>
     <row r="5" customHeight="1" spans="3:6">
-      <c r="C5" s="65" t="s">
+      <c r="C5" s="66" t="s">
         <v>0</v>
       </c>
-      <c r="D5" s="66"/>
-      <c r="E5" s="66"/>
-      <c r="F5" s="67"/>
+      <c r="D5" s="67"/>
+      <c r="E5" s="67"/>
+      <c r="F5" s="68"/>
     </row>
     <row r="6" customHeight="1" spans="3:6">
-      <c r="C6" s="68" t="s">
+      <c r="C6" s="69" t="s">
         <v>1</v>
       </c>
-      <c r="D6" s="69">
+      <c r="D6" s="70">
         <v>1</v>
       </c>
-      <c r="E6" s="70" t="s">
+      <c r="E6" s="71" t="s">
         <v>2</v>
       </c>
-      <c r="F6" s="79" t="s">
+      <c r="F6" s="80" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="7" customHeight="1" spans="3:6">
-      <c r="C7" s="68"/>
-      <c r="D7" s="69">
+      <c r="C7" s="69"/>
+      <c r="D7" s="70">
         <v>2</v>
       </c>
-      <c r="E7" s="70" t="s">
+      <c r="E7" s="71" t="s">
         <v>4</v>
       </c>
-      <c r="F7" s="79" t="s">
+      <c r="F7" s="80" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="8" customHeight="1" spans="3:6">
-      <c r="C8" s="68"/>
-      <c r="D8" s="69">
+      <c r="C8" s="69"/>
+      <c r="D8" s="70">
         <v>3</v>
       </c>
-      <c r="E8" s="70" t="s">
+      <c r="E8" s="71" t="s">
         <v>6</v>
       </c>
-      <c r="F8" s="79" t="s">
+      <c r="F8" s="80" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="9" customHeight="1" spans="3:6">
-      <c r="C9" s="68"/>
-      <c r="D9" s="69">
+      <c r="C9" s="69"/>
+      <c r="D9" s="70">
         <v>4</v>
       </c>
-      <c r="E9" s="70" t="s">
+      <c r="E9" s="71" t="s">
         <v>7</v>
       </c>
-      <c r="F9" s="71"/>
+      <c r="F9" s="72"/>
     </row>
     <row r="10" customHeight="1" spans="3:6">
-      <c r="C10" s="68"/>
-      <c r="D10" s="69">
+      <c r="C10" s="69"/>
+      <c r="D10" s="70">
         <v>5</v>
       </c>
-      <c r="E10" s="70" t="s">
+      <c r="E10" s="71" t="s">
         <v>8</v>
       </c>
-      <c r="F10" s="71"/>
+      <c r="F10" s="72"/>
     </row>
     <row r="11" customHeight="1" spans="3:6">
-      <c r="C11" s="72"/>
-      <c r="D11" s="73">
+      <c r="C11" s="73"/>
+      <c r="D11" s="74">
         <v>6</v>
       </c>
-      <c r="E11" s="74" t="s">
+      <c r="E11" s="75" t="s">
         <v>9</v>
       </c>
-      <c r="F11" s="75"/>
+      <c r="F11" s="76"/>
     </row>
     <row r="12" customHeight="1" spans="3:6">
-      <c r="C12" s="68" t="s">
+      <c r="C12" s="69" t="s">
         <v>10</v>
       </c>
-      <c r="D12" s="70">
+      <c r="D12" s="71">
         <v>1</v>
       </c>
-      <c r="E12" s="70" t="s">
+      <c r="E12" s="71" t="s">
         <v>11</v>
       </c>
-      <c r="F12" s="79" t="s">
+      <c r="F12" s="80" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="13" customHeight="1" spans="3:6">
-      <c r="C13" s="68"/>
-      <c r="D13" s="70">
+      <c r="C13" s="69"/>
+      <c r="D13" s="71">
         <v>2</v>
       </c>
-      <c r="E13" s="70" t="s">
+      <c r="E13" s="71" t="s">
         <v>13</v>
       </c>
-      <c r="F13" s="79" t="s">
+      <c r="F13" s="80" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="14" customHeight="1" spans="3:6">
-      <c r="C14" s="68"/>
-      <c r="D14" s="70">
+      <c r="C14" s="69"/>
+      <c r="D14" s="71">
         <v>3</v>
       </c>
-      <c r="E14" s="70" t="s">
+      <c r="E14" s="71" t="s">
         <v>14</v>
       </c>
-      <c r="F14" s="79" t="s">
+      <c r="F14" s="80" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="15" customHeight="1" spans="3:6">
-      <c r="C15" s="68"/>
-      <c r="D15" s="70">
+      <c r="C15" s="69"/>
+      <c r="D15" s="71">
         <v>4</v>
       </c>
-      <c r="E15" s="70" t="s">
+      <c r="E15" s="71" t="s">
         <v>15</v>
       </c>
-      <c r="F15" s="79" t="s">
+      <c r="F15" s="80" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="16" customHeight="1" spans="3:6">
-      <c r="C16" s="68"/>
-      <c r="D16" s="70">
+      <c r="C16" s="69"/>
+      <c r="D16" s="71">
         <v>5</v>
       </c>
-      <c r="E16" s="70" t="s">
+      <c r="E16" s="71" t="s">
         <v>17</v>
       </c>
-      <c r="F16" s="79" t="s">
+      <c r="F16" s="80" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="17" customHeight="1" spans="3:6">
-      <c r="C17" s="68"/>
-      <c r="D17" s="70">
+      <c r="C17" s="69"/>
+      <c r="D17" s="71">
         <v>6</v>
       </c>
-      <c r="E17" s="70" t="s">
+      <c r="E17" s="71" t="s">
         <v>18</v>
       </c>
-      <c r="F17" s="79" t="s">
+      <c r="F17" s="80" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="18" customHeight="1" spans="3:6">
-      <c r="C18" s="68"/>
-      <c r="D18" s="70">
+      <c r="C18" s="69"/>
+      <c r="D18" s="71">
         <v>7</v>
       </c>
-      <c r="E18" s="70" t="s">
+      <c r="E18" s="71" t="s">
         <v>7</v>
       </c>
-      <c r="F18" s="71"/>
+      <c r="F18" s="72"/>
     </row>
     <row r="19" customHeight="1" spans="3:6">
-      <c r="C19" s="68"/>
-      <c r="D19" s="70">
+      <c r="C19" s="69"/>
+      <c r="D19" s="71">
         <v>8</v>
       </c>
-      <c r="E19" s="64" t="s">
+      <c r="E19" s="65" t="s">
         <v>8</v>
       </c>
-      <c r="F19" s="71"/>
+      <c r="F19" s="72"/>
     </row>
     <row r="20" customHeight="1" spans="3:6">
-      <c r="C20" s="76"/>
-      <c r="D20" s="77">
+      <c r="C20" s="77"/>
+      <c r="D20" s="78">
         <v>9</v>
       </c>
-      <c r="E20" s="77" t="s">
+      <c r="E20" s="78" t="s">
         <v>9</v>
       </c>
-      <c r="F20" s="78"/>
+      <c r="F20" s="79"/>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -2422,291 +2447,291 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="8.55555555555556" style="29" customWidth="1"/>
-    <col min="2" max="2" width="3.88888888888889" style="39" customWidth="1"/>
-    <col min="3" max="3" width="3.44444444444444" style="29" customWidth="1"/>
-    <col min="4" max="4" width="6.77777777777778" style="29" customWidth="1"/>
-    <col min="5" max="5" width="12.3333333333333" style="29" customWidth="1"/>
-    <col min="6" max="6" width="8.44444444444444" style="29" customWidth="1"/>
-    <col min="7" max="7" width="9.33333333333333" style="39" customWidth="1"/>
-    <col min="8" max="8" width="6.66666666666667" style="29" customWidth="1"/>
-    <col min="9" max="9" width="8.88888888888889" style="29"/>
-    <col min="10" max="10" width="3.22222222222222" style="29" customWidth="1"/>
-    <col min="11" max="16384" width="8.88888888888889" style="29"/>
+    <col min="1" max="1" width="8.55555555555556" style="30" customWidth="1"/>
+    <col min="2" max="2" width="3.88888888888889" style="40" customWidth="1"/>
+    <col min="3" max="3" width="3.44444444444444" style="30" customWidth="1"/>
+    <col min="4" max="4" width="6.77777777777778" style="30" customWidth="1"/>
+    <col min="5" max="5" width="12.3333333333333" style="30" customWidth="1"/>
+    <col min="6" max="6" width="8.44444444444444" style="30" customWidth="1"/>
+    <col min="7" max="7" width="9.33333333333333" style="40" customWidth="1"/>
+    <col min="8" max="8" width="6.66666666666667" style="30" customWidth="1"/>
+    <col min="9" max="9" width="8.88888888888889" style="30"/>
+    <col min="10" max="10" width="3.22222222222222" style="30" customWidth="1"/>
+    <col min="11" max="16384" width="8.88888888888889" style="30"/>
   </cols>
   <sheetData>
     <row r="3" spans="2:10">
-      <c r="B3" s="40"/>
-      <c r="C3" s="41"/>
-      <c r="D3" s="41"/>
-      <c r="E3" s="41"/>
-      <c r="F3" s="41"/>
-      <c r="G3" s="42"/>
-      <c r="H3" s="41"/>
-      <c r="I3" s="41"/>
-      <c r="J3" s="57"/>
+      <c r="B3" s="41"/>
+      <c r="C3" s="42"/>
+      <c r="D3" s="42"/>
+      <c r="E3" s="42"/>
+      <c r="F3" s="42"/>
+      <c r="G3" s="43"/>
+      <c r="H3" s="42"/>
+      <c r="I3" s="42"/>
+      <c r="J3" s="58"/>
     </row>
     <row r="4" ht="19" customHeight="1" spans="2:10">
-      <c r="B4" s="43"/>
-      <c r="C4" s="44" t="s">
+      <c r="B4" s="44"/>
+      <c r="C4" s="45" t="s">
         <v>19</v>
       </c>
-      <c r="D4" s="44"/>
-      <c r="E4" s="44"/>
-      <c r="F4" s="44"/>
-      <c r="G4" s="44"/>
-      <c r="H4" s="44"/>
-      <c r="I4" s="44"/>
-      <c r="J4" s="58"/>
+      <c r="D4" s="45"/>
+      <c r="E4" s="45"/>
+      <c r="F4" s="45"/>
+      <c r="G4" s="45"/>
+      <c r="H4" s="45"/>
+      <c r="I4" s="45"/>
+      <c r="J4" s="59"/>
     </row>
     <row r="5" ht="18" customHeight="1" spans="2:10">
-      <c r="B5" s="43"/>
-      <c r="C5" s="39"/>
-      <c r="G5" s="39" t="s">
+      <c r="B5" s="44"/>
+      <c r="C5" s="40"/>
+      <c r="G5" s="40" t="s">
         <v>20</v>
       </c>
-      <c r="H5" s="39"/>
-      <c r="I5" s="39"/>
-      <c r="J5" s="58"/>
+      <c r="H5" s="40"/>
+      <c r="I5" s="40"/>
+      <c r="J5" s="59"/>
     </row>
     <row r="6" ht="16" customHeight="1" spans="2:10">
-      <c r="B6" s="43"/>
-      <c r="C6" s="39"/>
-      <c r="G6" s="29"/>
-      <c r="H6" s="39"/>
-      <c r="J6" s="58"/>
+      <c r="B6" s="44"/>
+      <c r="C6" s="40"/>
+      <c r="G6" s="30"/>
+      <c r="H6" s="40"/>
+      <c r="J6" s="59"/>
     </row>
     <row r="7" ht="15.15" spans="2:10">
-      <c r="B7" s="43"/>
-      <c r="C7" s="39"/>
-      <c r="D7" s="45" t="s">
+      <c r="B7" s="44"/>
+      <c r="C7" s="40"/>
+      <c r="D7" s="46" t="s">
         <v>21</v>
       </c>
-      <c r="E7" s="45"/>
-      <c r="F7" s="45"/>
-      <c r="G7" s="45"/>
-      <c r="H7" s="39"/>
-      <c r="I7" s="45"/>
-      <c r="J7" s="58"/>
+      <c r="E7" s="46"/>
+      <c r="F7" s="46"/>
+      <c r="G7" s="46"/>
+      <c r="H7" s="40"/>
+      <c r="I7" s="46"/>
+      <c r="J7" s="59"/>
     </row>
     <row r="8" ht="29.55" spans="2:10">
-      <c r="B8" s="43"/>
-      <c r="C8" s="46" t="s">
+      <c r="B8" s="44"/>
+      <c r="C8" s="47" t="s">
         <v>22</v>
       </c>
-      <c r="D8" s="47" t="s">
+      <c r="D8" s="48" t="s">
         <v>23</v>
       </c>
-      <c r="E8" s="47" t="s">
+      <c r="E8" s="48" t="s">
         <v>24</v>
       </c>
-      <c r="F8" s="47" t="s">
+      <c r="F8" s="48" t="s">
         <v>25</v>
       </c>
-      <c r="G8" s="47" t="s">
+      <c r="G8" s="48" t="s">
         <v>26</v>
       </c>
-      <c r="H8" s="48" t="s">
+      <c r="H8" s="49" t="s">
         <v>27</v>
       </c>
-      <c r="I8" s="59" t="s">
+      <c r="I8" s="60" t="s">
         <v>28</v>
       </c>
-      <c r="J8" s="58"/>
+      <c r="J8" s="59"/>
     </row>
     <row r="9" spans="2:10">
-      <c r="B9" s="43"/>
-      <c r="C9" s="49">
+      <c r="B9" s="44"/>
+      <c r="C9" s="50">
         <v>1</v>
       </c>
-      <c r="D9" s="37"/>
-      <c r="E9" s="37"/>
-      <c r="F9" s="37"/>
-      <c r="G9" s="37"/>
-      <c r="H9" s="80" t="s">
+      <c r="D9" s="38"/>
+      <c r="E9" s="38"/>
+      <c r="F9" s="38"/>
+      <c r="G9" s="38"/>
+      <c r="H9" s="81" t="s">
         <v>29</v>
       </c>
-      <c r="I9" s="60"/>
-      <c r="J9" s="58"/>
+      <c r="I9" s="61"/>
+      <c r="J9" s="59"/>
     </row>
     <row r="10" spans="2:10">
-      <c r="B10" s="43"/>
-      <c r="C10" s="51">
+      <c r="B10" s="44"/>
+      <c r="C10" s="52">
         <v>2</v>
       </c>
-      <c r="D10" s="52"/>
-      <c r="E10" s="52"/>
-      <c r="F10" s="52"/>
-      <c r="G10" s="52"/>
-      <c r="H10" s="80" t="s">
+      <c r="D10" s="53"/>
+      <c r="E10" s="53"/>
+      <c r="F10" s="53"/>
+      <c r="G10" s="53"/>
+      <c r="H10" s="81" t="s">
         <v>29</v>
       </c>
-      <c r="I10" s="61"/>
-      <c r="J10" s="58"/>
+      <c r="I10" s="62"/>
+      <c r="J10" s="59"/>
     </row>
     <row r="11" spans="2:10">
-      <c r="B11" s="43"/>
-      <c r="C11" s="51">
+      <c r="B11" s="44"/>
+      <c r="C11" s="52">
         <v>3</v>
       </c>
-      <c r="D11" s="52"/>
-      <c r="E11" s="52"/>
-      <c r="F11" s="52"/>
-      <c r="G11" s="52"/>
-      <c r="H11" s="80" t="s">
+      <c r="D11" s="53"/>
+      <c r="E11" s="53"/>
+      <c r="F11" s="53"/>
+      <c r="G11" s="53"/>
+      <c r="H11" s="81" t="s">
         <v>29</v>
       </c>
-      <c r="I11" s="61"/>
-      <c r="J11" s="58"/>
+      <c r="I11" s="62"/>
+      <c r="J11" s="59"/>
     </row>
     <row r="12" spans="2:10">
-      <c r="B12" s="43"/>
-      <c r="C12" s="51">
+      <c r="B12" s="44"/>
+      <c r="C12" s="52">
         <v>4</v>
       </c>
-      <c r="D12" s="52"/>
-      <c r="E12" s="52"/>
-      <c r="F12" s="52"/>
-      <c r="G12" s="52"/>
-      <c r="H12" s="80" t="s">
+      <c r="D12" s="53"/>
+      <c r="E12" s="53"/>
+      <c r="F12" s="53"/>
+      <c r="G12" s="53"/>
+      <c r="H12" s="81" t="s">
         <v>29</v>
       </c>
-      <c r="I12" s="61"/>
-      <c r="J12" s="58"/>
+      <c r="I12" s="62"/>
+      <c r="J12" s="59"/>
     </row>
     <row r="13" spans="2:10">
-      <c r="B13" s="43"/>
-      <c r="C13" s="51">
+      <c r="B13" s="44"/>
+      <c r="C13" s="52">
         <v>5</v>
       </c>
-      <c r="D13" s="52"/>
-      <c r="E13" s="52"/>
-      <c r="F13" s="52"/>
-      <c r="G13" s="52"/>
-      <c r="H13" s="80" t="s">
+      <c r="D13" s="53"/>
+      <c r="E13" s="53"/>
+      <c r="F13" s="53"/>
+      <c r="G13" s="53"/>
+      <c r="H13" s="81" t="s">
         <v>29</v>
       </c>
-      <c r="I13" s="61"/>
-      <c r="J13" s="58"/>
+      <c r="I13" s="62"/>
+      <c r="J13" s="59"/>
     </row>
     <row r="14" spans="2:10">
-      <c r="B14" s="43"/>
-      <c r="C14" s="51">
+      <c r="B14" s="44"/>
+      <c r="C14" s="52">
         <v>6</v>
       </c>
-      <c r="D14" s="52"/>
-      <c r="E14" s="52"/>
-      <c r="F14" s="52"/>
-      <c r="G14" s="52"/>
-      <c r="H14" s="80" t="s">
+      <c r="D14" s="53"/>
+      <c r="E14" s="53"/>
+      <c r="F14" s="53"/>
+      <c r="G14" s="53"/>
+      <c r="H14" s="81" t="s">
         <v>29</v>
       </c>
-      <c r="I14" s="61"/>
-      <c r="J14" s="58"/>
+      <c r="I14" s="62"/>
+      <c r="J14" s="59"/>
     </row>
     <row r="15" ht="15.15" spans="2:10">
-      <c r="B15" s="43"/>
-      <c r="C15" s="53"/>
-      <c r="D15" s="33"/>
-      <c r="E15" s="33"/>
-      <c r="F15" s="33"/>
-      <c r="G15" s="33"/>
-      <c r="H15" s="80" t="s">
+      <c r="B15" s="44"/>
+      <c r="C15" s="54"/>
+      <c r="D15" s="34"/>
+      <c r="E15" s="34"/>
+      <c r="F15" s="34"/>
+      <c r="G15" s="34"/>
+      <c r="H15" s="81" t="s">
         <v>29</v>
       </c>
-      <c r="I15" s="62"/>
-      <c r="J15" s="58"/>
+      <c r="I15" s="63"/>
+      <c r="J15" s="59"/>
     </row>
     <row r="16" ht="15.15" spans="2:10">
-      <c r="B16" s="43"/>
-      <c r="C16" s="46" t="s">
+      <c r="B16" s="44"/>
+      <c r="C16" s="47" t="s">
         <v>30</v>
       </c>
-      <c r="D16" s="47"/>
-      <c r="E16" s="47"/>
-      <c r="F16" s="47"/>
-      <c r="G16" s="47"/>
-      <c r="H16" s="48"/>
-      <c r="I16" s="81" t="s">
+      <c r="D16" s="48"/>
+      <c r="E16" s="48"/>
+      <c r="F16" s="48"/>
+      <c r="G16" s="48"/>
+      <c r="H16" s="49"/>
+      <c r="I16" s="82" t="s">
         <v>29</v>
       </c>
-      <c r="J16" s="58"/>
+      <c r="J16" s="59"/>
     </row>
     <row r="17" spans="2:10">
-      <c r="B17" s="54"/>
-      <c r="C17" s="55"/>
-      <c r="D17" s="55"/>
-      <c r="E17" s="55"/>
-      <c r="F17" s="55"/>
-      <c r="G17" s="56"/>
-      <c r="H17" s="55"/>
-      <c r="I17" s="55"/>
-      <c r="J17" s="63"/>
+      <c r="B17" s="55"/>
+      <c r="C17" s="56"/>
+      <c r="D17" s="56"/>
+      <c r="E17" s="56"/>
+      <c r="F17" s="56"/>
+      <c r="G17" s="57"/>
+      <c r="H17" s="56"/>
+      <c r="I17" s="56"/>
+      <c r="J17" s="64"/>
     </row>
     <row r="18" ht="17" customHeight="1"/>
     <row r="19" ht="13" customHeight="1" spans="12:13">
-      <c r="L19" s="29">
+      <c r="L19" s="30">
         <v>1</v>
       </c>
-      <c r="M19" s="29">
+      <c r="M19" s="30">
         <v>2</v>
       </c>
     </row>
     <row r="20" spans="12:15">
-      <c r="L20" s="29">
+      <c r="L20" s="30">
         <v>2</v>
       </c>
-      <c r="M20" s="29">
+      <c r="M20" s="30">
         <v>3</v>
       </c>
-      <c r="N20" s="29">
+      <c r="N20" s="30">
         <v>4</v>
       </c>
-      <c r="O20" s="29">
+      <c r="O20" s="30">
         <v>5</v>
       </c>
     </row>
     <row r="21" spans="13:15">
-      <c r="M21" s="29">
+      <c r="M21" s="30">
         <v>4</v>
       </c>
-      <c r="O21" s="29">
+      <c r="O21" s="30">
         <v>6</v>
       </c>
     </row>
     <row r="22" spans="13:15">
-      <c r="M22" s="29">
+      <c r="M22" s="30">
         <v>5</v>
       </c>
-      <c r="N22" s="29">
+      <c r="N22" s="30">
         <v>6</v>
       </c>
-      <c r="O22" s="29">
+      <c r="O22" s="30">
         <v>7</v>
       </c>
     </row>
     <row r="23" spans="14:14">
-      <c r="N23" s="29">
+      <c r="N23" s="30">
         <v>8</v>
       </c>
     </row>
     <row r="25" spans="14:14">
-      <c r="N25" s="29">
+      <c r="N25" s="30">
         <v>10</v>
       </c>
     </row>
     <row r="26" spans="14:14">
-      <c r="N26" s="29">
+      <c r="N26" s="30">
         <v>12</v>
       </c>
     </row>
     <row r="28" spans="14:14">
-      <c r="N28" s="29">
+      <c r="N28" s="30">
         <v>14</v>
       </c>
     </row>
     <row r="29" spans="14:14">
-      <c r="N29" s="29">
+      <c r="N29" s="30">
         <v>16</v>
       </c>
     </row>
@@ -2727,79 +2752,79 @@
   <sheetPr/>
   <dimension ref="B5:E10"/>
   <sheetViews>
-    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="14.4" outlineLevelCol="4"/>
   <cols>
-    <col min="1" max="1" width="13.4444444444444" style="29" customWidth="1"/>
-    <col min="2" max="2" width="17.8888888888889" style="29" customWidth="1"/>
-    <col min="3" max="4" width="31" style="29" customWidth="1"/>
-    <col min="5" max="5" width="20.1944444444444" style="29" customWidth="1"/>
-    <col min="6" max="16384" width="8.88888888888889" style="29"/>
+    <col min="1" max="1" width="13.4444444444444" style="30" customWidth="1"/>
+    <col min="2" max="2" width="17.8888888888889" style="30" customWidth="1"/>
+    <col min="3" max="4" width="31" style="30" customWidth="1"/>
+    <col min="5" max="5" width="20.1944444444444" style="30" customWidth="1"/>
+    <col min="6" max="16384" width="8.88888888888889" style="30"/>
   </cols>
   <sheetData>
     <row r="5" ht="15.6" spans="2:4">
-      <c r="B5" s="30" t="s">
+      <c r="B5" s="31" t="s">
         <v>31</v>
       </c>
-      <c r="C5" s="30"/>
-      <c r="D5" s="30"/>
+      <c r="C5" s="31"/>
+      <c r="D5" s="31"/>
     </row>
     <row r="6" spans="2:5">
-      <c r="B6" s="31" t="s">
+      <c r="B6" s="32" t="s">
         <v>32</v>
       </c>
-      <c r="C6" s="31" t="s">
+      <c r="C6" s="32" t="s">
         <v>33</v>
       </c>
-      <c r="D6" s="31" t="s">
+      <c r="D6" s="32" t="s">
         <v>34</v>
       </c>
-      <c r="E6" s="32"/>
+      <c r="E6" s="33"/>
     </row>
     <row r="7" ht="16" customHeight="1" spans="2:4">
-      <c r="B7" s="33" t="s">
+      <c r="B7" s="34" t="s">
         <v>35</v>
       </c>
-      <c r="C7" s="34" t="s">
+      <c r="C7" s="35" t="s">
         <v>36</v>
       </c>
-      <c r="D7" s="34" t="s">
+      <c r="D7" s="35" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="8" ht="16" customHeight="1" spans="2:4">
-      <c r="B8" s="35" t="s">
+      <c r="B8" s="36" t="s">
         <v>38</v>
       </c>
-      <c r="C8" s="34" t="s">
+      <c r="C8" s="35" t="s">
         <v>39</v>
       </c>
-      <c r="D8" s="34" t="s">
+      <c r="D8" s="35" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="9" ht="16" customHeight="1" spans="2:4">
-      <c r="B9" s="36" t="s">
+      <c r="B9" s="37" t="s">
         <v>41</v>
       </c>
-      <c r="C9" s="34" t="s">
+      <c r="C9" s="35" t="s">
         <v>42</v>
       </c>
-      <c r="D9" s="34" t="s">
+      <c r="D9" s="35" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="10" ht="16" customHeight="1" spans="2:4">
-      <c r="B10" s="37" t="s">
+      <c r="B10" s="38" t="s">
         <v>44</v>
       </c>
-      <c r="C10" s="38" t="s">
+      <c r="C10" s="39" t="s">
         <v>42</v>
       </c>
-      <c r="D10" s="38" t="s">
+      <c r="D10" s="39" t="s">
         <v>45</v>
       </c>
     </row>
@@ -2817,13 +2842,14 @@
   <sheetPr/>
   <dimension ref="C4:K11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N7" sqref="N7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="N3" sqref="N3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="14.4"/>
   <cols>
     <col min="3" max="9" width="10.7777777777778" customWidth="1"/>
+    <col min="11" max="11" width="10.2222222222222" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="4" ht="15.15"/>
@@ -2836,7 +2862,7 @@
       <c r="F5" s="3"/>
       <c r="G5" s="3"/>
       <c r="H5" s="3"/>
-      <c r="I5" s="20"/>
+      <c r="I5" s="21"/>
     </row>
     <row r="6" s="1" customFormat="1" ht="18" customHeight="1" spans="3:9">
       <c r="C6" s="4" t="s">
@@ -2880,10 +2906,10 @@
       <c r="H7" s="9">
         <v>6</v>
       </c>
-      <c r="I7" s="21">
+      <c r="I7" s="22">
         <v>7</v>
       </c>
-      <c r="K7" s="22" t="s">
+      <c r="K7" s="23" t="s">
         <v>54</v>
       </c>
     </row>
@@ -2906,10 +2932,10 @@
       <c r="H8" s="11">
         <v>13</v>
       </c>
-      <c r="I8" s="23">
+      <c r="I8" s="24">
         <v>14</v>
       </c>
-      <c r="K8" s="24" t="s">
+      <c r="K8" s="25" t="s">
         <v>55</v>
       </c>
     </row>
@@ -2917,30 +2943,30 @@
       <c r="C9" s="15">
         <v>15</v>
       </c>
-      <c r="D9" s="16">
+      <c r="D9" s="14">
         <v>16</v>
       </c>
-      <c r="E9" s="16">
+      <c r="E9" s="14">
         <v>17</v>
       </c>
-      <c r="F9" s="16">
+      <c r="F9" s="14">
         <v>18</v>
       </c>
-      <c r="G9" s="16">
+      <c r="G9" s="11">
         <v>19</v>
       </c>
       <c r="H9" s="16">
         <v>20</v>
       </c>
-      <c r="I9" s="25">
+      <c r="I9" s="26">
         <v>21</v>
       </c>
-      <c r="K9" s="26" t="s">
+      <c r="K9" s="27" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="10" ht="52" customHeight="1" spans="3:11">
-      <c r="C10" s="15">
+      <c r="C10" s="17">
         <v>22</v>
       </c>
       <c r="D10" s="16">
@@ -2958,33 +2984,33 @@
       <c r="H10" s="16">
         <v>27</v>
       </c>
-      <c r="I10" s="25">
+      <c r="I10" s="26">
         <v>28</v>
       </c>
-      <c r="K10" s="27" t="s">
+      <c r="K10" s="28" t="s">
         <v>57</v>
       </c>
     </row>
     <row r="11" ht="52" customHeight="1" spans="3:9">
-      <c r="C11" s="17">
+      <c r="C11" s="18">
         <v>29</v>
       </c>
-      <c r="D11" s="18">
+      <c r="D11" s="19">
         <v>30</v>
       </c>
-      <c r="E11" s="19">
+      <c r="E11" s="20">
         <v>1</v>
       </c>
-      <c r="F11" s="19">
+      <c r="F11" s="20">
         <v>2</v>
       </c>
-      <c r="G11" s="19">
+      <c r="G11" s="20">
         <v>3</v>
       </c>
-      <c r="H11" s="19">
+      <c r="H11" s="20">
         <v>4</v>
       </c>
-      <c r="I11" s="28">
+      <c r="I11" s="29">
         <v>5</v>
       </c>
     </row>

</xml_diff>

<commit_message>
admin -> input output user supplier product stock selling purchase
</commit_message>
<xml_diff>
--- a/myfile/Information.xlsx
+++ b/myfile/Information.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="23040" windowHeight="9204" activeTab="2"/>
+    <workbookView windowWidth="23040" windowHeight="9204" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Rules" sheetId="2" r:id="rId1"/>
@@ -475,9 +475,9 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
     <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
   <fonts count="27">
     <font>
@@ -525,6 +525,13 @@
     </font>
     <font>
       <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
@@ -532,14 +539,15 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C6500"/>
+      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color theme="0"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -553,6 +561,14 @@
     </font>
     <font>
       <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
@@ -561,10 +577,10 @@
     </font>
     <font>
       <b/>
-      <sz val="13"/>
-      <color theme="3"/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
-      <charset val="134"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -593,7 +609,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF3F3F76"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -615,9 +631,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
+      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -631,14 +646,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color rgb="FF006100"/>
       <name val="Calibri"/>
@@ -647,7 +654,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -655,14 +662,7 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
+      <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -712,31 +712,157 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="7" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFFFEB9C"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -748,7 +874,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -760,139 +892,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1406,6 +1406,30 @@
       <top/>
       <bottom style="medium">
         <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1421,69 +1445,6 @@
       </top>
       <bottom style="double">
         <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1507,12 +1468,51 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -1530,134 +1530,134 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="9" borderId="43" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="14" borderId="45" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="44" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="22" borderId="48" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="24" borderId="49" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="44" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="48" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="44" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="46" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="16" borderId="45" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="20" borderId="47" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="33" borderId="43" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="10" borderId="50" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="10" borderId="43" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="47" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="46" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="20" borderId="45" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="50" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="49" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="80">
+  <cellXfs count="79">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1709,9 +1709,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
@@ -1736,11 +1733,11 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -2234,196 +2231,196 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="16" customHeight="1" outlineLevelCol="5"/>
   <cols>
-    <col min="1" max="3" width="8.88888888888889" style="30"/>
-    <col min="4" max="4" width="3.44444444444444" style="30" customWidth="1"/>
-    <col min="5" max="5" width="31.6666666666667" style="30" customWidth="1"/>
-    <col min="6" max="6" width="21" style="30" customWidth="1"/>
-    <col min="7" max="16384" width="8.88888888888889" style="30"/>
+    <col min="1" max="3" width="8.88888888888889" style="29"/>
+    <col min="4" max="4" width="3.44444444444444" style="29" customWidth="1"/>
+    <col min="5" max="5" width="31.6666666666667" style="29" customWidth="1"/>
+    <col min="6" max="6" width="21" style="29" customWidth="1"/>
+    <col min="7" max="16384" width="8.88888888888889" style="29"/>
   </cols>
   <sheetData>
     <row r="4" customHeight="1" spans="3:4">
-      <c r="C4" s="65"/>
-      <c r="D4" s="65"/>
+      <c r="C4" s="64"/>
+      <c r="D4" s="64"/>
     </row>
     <row r="5" customHeight="1" spans="3:6">
-      <c r="C5" s="66" t="s">
+      <c r="C5" s="65" t="s">
         <v>0</v>
       </c>
-      <c r="D5" s="67"/>
-      <c r="E5" s="67"/>
-      <c r="F5" s="68"/>
+      <c r="D5" s="66"/>
+      <c r="E5" s="66"/>
+      <c r="F5" s="67"/>
     </row>
     <row r="6" customHeight="1" spans="3:6">
-      <c r="C6" s="69" t="s">
+      <c r="C6" s="68" t="s">
         <v>1</v>
       </c>
-      <c r="D6" s="70">
+      <c r="D6" s="69">
         <v>1</v>
       </c>
-      <c r="E6" s="71" t="s">
+      <c r="E6" s="70" t="s">
         <v>2</v>
       </c>
-      <c r="F6" s="80" t="s">
+      <c r="F6" s="79" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="7" customHeight="1" spans="3:6">
-      <c r="C7" s="69"/>
-      <c r="D7" s="70">
+      <c r="C7" s="68"/>
+      <c r="D7" s="69">
         <v>2</v>
       </c>
-      <c r="E7" s="71" t="s">
+      <c r="E7" s="70" t="s">
         <v>4</v>
       </c>
-      <c r="F7" s="80" t="s">
+      <c r="F7" s="79" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="8" customHeight="1" spans="3:6">
-      <c r="C8" s="69"/>
-      <c r="D8" s="70">
+      <c r="C8" s="68"/>
+      <c r="D8" s="69">
         <v>3</v>
       </c>
-      <c r="E8" s="71" t="s">
+      <c r="E8" s="70" t="s">
         <v>6</v>
       </c>
-      <c r="F8" s="80" t="s">
+      <c r="F8" s="79" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="9" customHeight="1" spans="3:6">
-      <c r="C9" s="69"/>
-      <c r="D9" s="70">
+      <c r="C9" s="68"/>
+      <c r="D9" s="69">
         <v>4</v>
       </c>
-      <c r="E9" s="71" t="s">
+      <c r="E9" s="70" t="s">
         <v>7</v>
       </c>
-      <c r="F9" s="72"/>
+      <c r="F9" s="71"/>
     </row>
     <row r="10" customHeight="1" spans="3:6">
-      <c r="C10" s="69"/>
-      <c r="D10" s="70">
+      <c r="C10" s="68"/>
+      <c r="D10" s="69">
         <v>5</v>
       </c>
-      <c r="E10" s="71" t="s">
+      <c r="E10" s="70" t="s">
         <v>8</v>
       </c>
-      <c r="F10" s="72"/>
+      <c r="F10" s="71"/>
     </row>
     <row r="11" customHeight="1" spans="3:6">
-      <c r="C11" s="73"/>
-      <c r="D11" s="74">
+      <c r="C11" s="72"/>
+      <c r="D11" s="73">
         <v>6</v>
       </c>
-      <c r="E11" s="75" t="s">
+      <c r="E11" s="74" t="s">
         <v>9</v>
       </c>
-      <c r="F11" s="76"/>
+      <c r="F11" s="75"/>
     </row>
     <row r="12" customHeight="1" spans="3:6">
-      <c r="C12" s="69" t="s">
+      <c r="C12" s="68" t="s">
         <v>10</v>
       </c>
-      <c r="D12" s="71">
+      <c r="D12" s="70">
         <v>1</v>
       </c>
-      <c r="E12" s="71" t="s">
+      <c r="E12" s="70" t="s">
         <v>11</v>
       </c>
-      <c r="F12" s="80" t="s">
+      <c r="F12" s="79" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="13" customHeight="1" spans="3:6">
-      <c r="C13" s="69"/>
-      <c r="D13" s="71">
+      <c r="C13" s="68"/>
+      <c r="D13" s="70">
         <v>2</v>
       </c>
-      <c r="E13" s="71" t="s">
+      <c r="E13" s="70" t="s">
         <v>13</v>
       </c>
-      <c r="F13" s="80" t="s">
+      <c r="F13" s="79" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="14" customHeight="1" spans="3:6">
-      <c r="C14" s="69"/>
-      <c r="D14" s="71">
+      <c r="C14" s="68"/>
+      <c r="D14" s="70">
         <v>3</v>
       </c>
-      <c r="E14" s="71" t="s">
+      <c r="E14" s="70" t="s">
         <v>14</v>
       </c>
-      <c r="F14" s="80" t="s">
+      <c r="F14" s="79" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="15" customHeight="1" spans="3:6">
-      <c r="C15" s="69"/>
-      <c r="D15" s="71">
+      <c r="C15" s="68"/>
+      <c r="D15" s="70">
         <v>4</v>
       </c>
-      <c r="E15" s="71" t="s">
+      <c r="E15" s="70" t="s">
         <v>15</v>
       </c>
-      <c r="F15" s="80" t="s">
+      <c r="F15" s="79" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="16" customHeight="1" spans="3:6">
-      <c r="C16" s="69"/>
-      <c r="D16" s="71">
+      <c r="C16" s="68"/>
+      <c r="D16" s="70">
         <v>5</v>
       </c>
-      <c r="E16" s="71" t="s">
+      <c r="E16" s="70" t="s">
         <v>17</v>
       </c>
-      <c r="F16" s="80" t="s">
+      <c r="F16" s="79" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="17" customHeight="1" spans="3:6">
-      <c r="C17" s="69"/>
-      <c r="D17" s="71">
+      <c r="C17" s="68"/>
+      <c r="D17" s="70">
         <v>6</v>
       </c>
-      <c r="E17" s="71" t="s">
+      <c r="E17" s="70" t="s">
         <v>18</v>
       </c>
-      <c r="F17" s="80" t="s">
+      <c r="F17" s="79" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="18" customHeight="1" spans="3:6">
-      <c r="C18" s="69"/>
-      <c r="D18" s="71">
+      <c r="C18" s="68"/>
+      <c r="D18" s="70">
         <v>7</v>
       </c>
-      <c r="E18" s="71" t="s">
+      <c r="E18" s="70" t="s">
         <v>7</v>
       </c>
-      <c r="F18" s="72"/>
+      <c r="F18" s="71"/>
     </row>
     <row r="19" customHeight="1" spans="3:6">
-      <c r="C19" s="69"/>
-      <c r="D19" s="71">
+      <c r="C19" s="68"/>
+      <c r="D19" s="70">
         <v>8</v>
       </c>
-      <c r="E19" s="65" t="s">
+      <c r="E19" s="64" t="s">
         <v>8</v>
       </c>
-      <c r="F19" s="72"/>
+      <c r="F19" s="71"/>
     </row>
     <row r="20" customHeight="1" spans="3:6">
-      <c r="C20" s="77"/>
-      <c r="D20" s="78">
+      <c r="C20" s="76"/>
+      <c r="D20" s="77">
         <v>9</v>
       </c>
-      <c r="E20" s="78" t="s">
+      <c r="E20" s="77" t="s">
         <v>9</v>
       </c>
-      <c r="F20" s="79"/>
+      <c r="F20" s="78"/>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -2447,291 +2444,291 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="8.55555555555556" style="30" customWidth="1"/>
-    <col min="2" max="2" width="3.88888888888889" style="40" customWidth="1"/>
-    <col min="3" max="3" width="3.44444444444444" style="30" customWidth="1"/>
-    <col min="4" max="4" width="6.77777777777778" style="30" customWidth="1"/>
-    <col min="5" max="5" width="12.3333333333333" style="30" customWidth="1"/>
-    <col min="6" max="6" width="8.44444444444444" style="30" customWidth="1"/>
-    <col min="7" max="7" width="9.33333333333333" style="40" customWidth="1"/>
-    <col min="8" max="8" width="6.66666666666667" style="30" customWidth="1"/>
-    <col min="9" max="9" width="8.88888888888889" style="30"/>
-    <col min="10" max="10" width="3.22222222222222" style="30" customWidth="1"/>
-    <col min="11" max="16384" width="8.88888888888889" style="30"/>
+    <col min="1" max="1" width="8.55555555555556" style="29" customWidth="1"/>
+    <col min="2" max="2" width="3.88888888888889" style="39" customWidth="1"/>
+    <col min="3" max="3" width="3.44444444444444" style="29" customWidth="1"/>
+    <col min="4" max="4" width="6.77777777777778" style="29" customWidth="1"/>
+    <col min="5" max="5" width="12.3333333333333" style="29" customWidth="1"/>
+    <col min="6" max="6" width="8.44444444444444" style="29" customWidth="1"/>
+    <col min="7" max="7" width="9.33333333333333" style="39" customWidth="1"/>
+    <col min="8" max="8" width="6.66666666666667" style="29" customWidth="1"/>
+    <col min="9" max="9" width="8.88888888888889" style="29"/>
+    <col min="10" max="10" width="3.22222222222222" style="29" customWidth="1"/>
+    <col min="11" max="16384" width="8.88888888888889" style="29"/>
   </cols>
   <sheetData>
     <row r="3" spans="2:10">
-      <c r="B3" s="41"/>
-      <c r="C3" s="42"/>
-      <c r="D3" s="42"/>
-      <c r="E3" s="42"/>
-      <c r="F3" s="42"/>
-      <c r="G3" s="43"/>
-      <c r="H3" s="42"/>
-      <c r="I3" s="42"/>
-      <c r="J3" s="58"/>
+      <c r="B3" s="40"/>
+      <c r="C3" s="41"/>
+      <c r="D3" s="41"/>
+      <c r="E3" s="41"/>
+      <c r="F3" s="41"/>
+      <c r="G3" s="42"/>
+      <c r="H3" s="41"/>
+      <c r="I3" s="41"/>
+      <c r="J3" s="57"/>
     </row>
     <row r="4" ht="19" customHeight="1" spans="2:10">
-      <c r="B4" s="44"/>
-      <c r="C4" s="45" t="s">
+      <c r="B4" s="43"/>
+      <c r="C4" s="44" t="s">
         <v>19</v>
       </c>
-      <c r="D4" s="45"/>
-      <c r="E4" s="45"/>
-      <c r="F4" s="45"/>
-      <c r="G4" s="45"/>
-      <c r="H4" s="45"/>
-      <c r="I4" s="45"/>
-      <c r="J4" s="59"/>
+      <c r="D4" s="44"/>
+      <c r="E4" s="44"/>
+      <c r="F4" s="44"/>
+      <c r="G4" s="44"/>
+      <c r="H4" s="44"/>
+      <c r="I4" s="44"/>
+      <c r="J4" s="58"/>
     </row>
     <row r="5" ht="18" customHeight="1" spans="2:10">
-      <c r="B5" s="44"/>
-      <c r="C5" s="40"/>
-      <c r="G5" s="40" t="s">
+      <c r="B5" s="43"/>
+      <c r="C5" s="39"/>
+      <c r="G5" s="39" t="s">
         <v>20</v>
       </c>
-      <c r="H5" s="40"/>
-      <c r="I5" s="40"/>
-      <c r="J5" s="59"/>
+      <c r="H5" s="39"/>
+      <c r="I5" s="39"/>
+      <c r="J5" s="58"/>
     </row>
     <row r="6" ht="16" customHeight="1" spans="2:10">
-      <c r="B6" s="44"/>
-      <c r="C6" s="40"/>
-      <c r="G6" s="30"/>
-      <c r="H6" s="40"/>
-      <c r="J6" s="59"/>
+      <c r="B6" s="43"/>
+      <c r="C6" s="39"/>
+      <c r="G6" s="29"/>
+      <c r="H6" s="39"/>
+      <c r="J6" s="58"/>
     </row>
     <row r="7" ht="15.15" spans="2:10">
-      <c r="B7" s="44"/>
-      <c r="C7" s="40"/>
-      <c r="D7" s="46" t="s">
+      <c r="B7" s="43"/>
+      <c r="C7" s="39"/>
+      <c r="D7" s="45" t="s">
         <v>21</v>
       </c>
-      <c r="E7" s="46"/>
-      <c r="F7" s="46"/>
-      <c r="G7" s="46"/>
-      <c r="H7" s="40"/>
-      <c r="I7" s="46"/>
-      <c r="J7" s="59"/>
+      <c r="E7" s="45"/>
+      <c r="F7" s="45"/>
+      <c r="G7" s="45"/>
+      <c r="H7" s="39"/>
+      <c r="I7" s="45"/>
+      <c r="J7" s="58"/>
     </row>
     <row r="8" ht="29.55" spans="2:10">
-      <c r="B8" s="44"/>
-      <c r="C8" s="47" t="s">
+      <c r="B8" s="43"/>
+      <c r="C8" s="46" t="s">
         <v>22</v>
       </c>
-      <c r="D8" s="48" t="s">
+      <c r="D8" s="47" t="s">
         <v>23</v>
       </c>
-      <c r="E8" s="48" t="s">
+      <c r="E8" s="47" t="s">
         <v>24</v>
       </c>
-      <c r="F8" s="48" t="s">
+      <c r="F8" s="47" t="s">
         <v>25</v>
       </c>
-      <c r="G8" s="48" t="s">
+      <c r="G8" s="47" t="s">
         <v>26</v>
       </c>
-      <c r="H8" s="49" t="s">
+      <c r="H8" s="48" t="s">
         <v>27</v>
       </c>
-      <c r="I8" s="60" t="s">
+      <c r="I8" s="59" t="s">
         <v>28</v>
       </c>
-      <c r="J8" s="59"/>
+      <c r="J8" s="58"/>
     </row>
     <row r="9" spans="2:10">
-      <c r="B9" s="44"/>
-      <c r="C9" s="50">
+      <c r="B9" s="43"/>
+      <c r="C9" s="49">
         <v>1</v>
       </c>
-      <c r="D9" s="38"/>
-      <c r="E9" s="38"/>
-      <c r="F9" s="38"/>
-      <c r="G9" s="38"/>
-      <c r="H9" s="81" t="s">
+      <c r="D9" s="37"/>
+      <c r="E9" s="37"/>
+      <c r="F9" s="37"/>
+      <c r="G9" s="37"/>
+      <c r="H9" s="80" t="s">
         <v>29</v>
       </c>
-      <c r="I9" s="61"/>
-      <c r="J9" s="59"/>
+      <c r="I9" s="60"/>
+      <c r="J9" s="58"/>
     </row>
     <row r="10" spans="2:10">
-      <c r="B10" s="44"/>
-      <c r="C10" s="52">
+      <c r="B10" s="43"/>
+      <c r="C10" s="51">
         <v>2</v>
       </c>
-      <c r="D10" s="53"/>
-      <c r="E10" s="53"/>
-      <c r="F10" s="53"/>
-      <c r="G10" s="53"/>
-      <c r="H10" s="81" t="s">
+      <c r="D10" s="52"/>
+      <c r="E10" s="52"/>
+      <c r="F10" s="52"/>
+      <c r="G10" s="52"/>
+      <c r="H10" s="80" t="s">
         <v>29</v>
       </c>
-      <c r="I10" s="62"/>
-      <c r="J10" s="59"/>
+      <c r="I10" s="61"/>
+      <c r="J10" s="58"/>
     </row>
     <row r="11" spans="2:10">
-      <c r="B11" s="44"/>
-      <c r="C11" s="52">
+      <c r="B11" s="43"/>
+      <c r="C11" s="51">
         <v>3</v>
       </c>
-      <c r="D11" s="53"/>
-      <c r="E11" s="53"/>
-      <c r="F11" s="53"/>
-      <c r="G11" s="53"/>
-      <c r="H11" s="81" t="s">
+      <c r="D11" s="52"/>
+      <c r="E11" s="52"/>
+      <c r="F11" s="52"/>
+      <c r="G11" s="52"/>
+      <c r="H11" s="80" t="s">
         <v>29</v>
       </c>
-      <c r="I11" s="62"/>
-      <c r="J11" s="59"/>
+      <c r="I11" s="61"/>
+      <c r="J11" s="58"/>
     </row>
     <row r="12" spans="2:10">
-      <c r="B12" s="44"/>
-      <c r="C12" s="52">
+      <c r="B12" s="43"/>
+      <c r="C12" s="51">
         <v>4</v>
       </c>
-      <c r="D12" s="53"/>
-      <c r="E12" s="53"/>
-      <c r="F12" s="53"/>
-      <c r="G12" s="53"/>
-      <c r="H12" s="81" t="s">
+      <c r="D12" s="52"/>
+      <c r="E12" s="52"/>
+      <c r="F12" s="52"/>
+      <c r="G12" s="52"/>
+      <c r="H12" s="80" t="s">
         <v>29</v>
       </c>
-      <c r="I12" s="62"/>
-      <c r="J12" s="59"/>
+      <c r="I12" s="61"/>
+      <c r="J12" s="58"/>
     </row>
     <row r="13" spans="2:10">
-      <c r="B13" s="44"/>
-      <c r="C13" s="52">
+      <c r="B13" s="43"/>
+      <c r="C13" s="51">
         <v>5</v>
       </c>
-      <c r="D13" s="53"/>
-      <c r="E13" s="53"/>
-      <c r="F13" s="53"/>
-      <c r="G13" s="53"/>
-      <c r="H13" s="81" t="s">
+      <c r="D13" s="52"/>
+      <c r="E13" s="52"/>
+      <c r="F13" s="52"/>
+      <c r="G13" s="52"/>
+      <c r="H13" s="80" t="s">
         <v>29</v>
       </c>
-      <c r="I13" s="62"/>
-      <c r="J13" s="59"/>
+      <c r="I13" s="61"/>
+      <c r="J13" s="58"/>
     </row>
     <row r="14" spans="2:10">
-      <c r="B14" s="44"/>
-      <c r="C14" s="52">
+      <c r="B14" s="43"/>
+      <c r="C14" s="51">
         <v>6</v>
       </c>
-      <c r="D14" s="53"/>
-      <c r="E14" s="53"/>
-      <c r="F14" s="53"/>
-      <c r="G14" s="53"/>
-      <c r="H14" s="81" t="s">
+      <c r="D14" s="52"/>
+      <c r="E14" s="52"/>
+      <c r="F14" s="52"/>
+      <c r="G14" s="52"/>
+      <c r="H14" s="80" t="s">
         <v>29</v>
       </c>
-      <c r="I14" s="62"/>
-      <c r="J14" s="59"/>
+      <c r="I14" s="61"/>
+      <c r="J14" s="58"/>
     </row>
     <row r="15" ht="15.15" spans="2:10">
-      <c r="B15" s="44"/>
-      <c r="C15" s="54"/>
-      <c r="D15" s="34"/>
-      <c r="E15" s="34"/>
-      <c r="F15" s="34"/>
-      <c r="G15" s="34"/>
-      <c r="H15" s="81" t="s">
+      <c r="B15" s="43"/>
+      <c r="C15" s="53"/>
+      <c r="D15" s="33"/>
+      <c r="E15" s="33"/>
+      <c r="F15" s="33"/>
+      <c r="G15" s="33"/>
+      <c r="H15" s="80" t="s">
         <v>29</v>
       </c>
-      <c r="I15" s="63"/>
-      <c r="J15" s="59"/>
+      <c r="I15" s="62"/>
+      <c r="J15" s="58"/>
     </row>
     <row r="16" ht="15.15" spans="2:10">
-      <c r="B16" s="44"/>
-      <c r="C16" s="47" t="s">
+      <c r="B16" s="43"/>
+      <c r="C16" s="46" t="s">
         <v>30</v>
       </c>
-      <c r="D16" s="48"/>
-      <c r="E16" s="48"/>
-      <c r="F16" s="48"/>
-      <c r="G16" s="48"/>
-      <c r="H16" s="49"/>
-      <c r="I16" s="82" t="s">
+      <c r="D16" s="47"/>
+      <c r="E16" s="47"/>
+      <c r="F16" s="47"/>
+      <c r="G16" s="47"/>
+      <c r="H16" s="48"/>
+      <c r="I16" s="81" t="s">
         <v>29</v>
       </c>
-      <c r="J16" s="59"/>
+      <c r="J16" s="58"/>
     </row>
     <row r="17" spans="2:10">
-      <c r="B17" s="55"/>
-      <c r="C17" s="56"/>
-      <c r="D17" s="56"/>
-      <c r="E17" s="56"/>
-      <c r="F17" s="56"/>
-      <c r="G17" s="57"/>
-      <c r="H17" s="56"/>
-      <c r="I17" s="56"/>
-      <c r="J17" s="64"/>
+      <c r="B17" s="54"/>
+      <c r="C17" s="55"/>
+      <c r="D17" s="55"/>
+      <c r="E17" s="55"/>
+      <c r="F17" s="55"/>
+      <c r="G17" s="56"/>
+      <c r="H17" s="55"/>
+      <c r="I17" s="55"/>
+      <c r="J17" s="63"/>
     </row>
     <row r="18" ht="17" customHeight="1"/>
     <row r="19" ht="13" customHeight="1" spans="12:13">
-      <c r="L19" s="30">
+      <c r="L19" s="29">
         <v>1</v>
       </c>
-      <c r="M19" s="30">
+      <c r="M19" s="29">
         <v>2</v>
       </c>
     </row>
     <row r="20" spans="12:15">
-      <c r="L20" s="30">
+      <c r="L20" s="29">
         <v>2</v>
       </c>
-      <c r="M20" s="30">
+      <c r="M20" s="29">
         <v>3</v>
       </c>
-      <c r="N20" s="30">
+      <c r="N20" s="29">
         <v>4</v>
       </c>
-      <c r="O20" s="30">
+      <c r="O20" s="29">
         <v>5</v>
       </c>
     </row>
     <row r="21" spans="13:15">
-      <c r="M21" s="30">
+      <c r="M21" s="29">
         <v>4</v>
       </c>
-      <c r="O21" s="30">
+      <c r="O21" s="29">
         <v>6</v>
       </c>
     </row>
     <row r="22" spans="13:15">
-      <c r="M22" s="30">
+      <c r="M22" s="29">
         <v>5</v>
       </c>
-      <c r="N22" s="30">
+      <c r="N22" s="29">
         <v>6</v>
       </c>
-      <c r="O22" s="30">
+      <c r="O22" s="29">
         <v>7</v>
       </c>
     </row>
     <row r="23" spans="14:14">
-      <c r="N23" s="30">
+      <c r="N23" s="29">
         <v>8</v>
       </c>
     </row>
     <row r="25" spans="14:14">
-      <c r="N25" s="30">
+      <c r="N25" s="29">
         <v>10</v>
       </c>
     </row>
     <row r="26" spans="14:14">
-      <c r="N26" s="30">
+      <c r="N26" s="29">
         <v>12</v>
       </c>
     </row>
     <row r="28" spans="14:14">
-      <c r="N28" s="30">
+      <c r="N28" s="29">
         <v>14</v>
       </c>
     </row>
     <row r="29" spans="14:14">
-      <c r="N29" s="30">
+      <c r="N29" s="29">
         <v>16</v>
       </c>
     </row>
@@ -2752,79 +2749,79 @@
   <sheetPr/>
   <dimension ref="B5:E10"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="14.4" outlineLevelCol="4"/>
   <cols>
-    <col min="1" max="1" width="13.4444444444444" style="30" customWidth="1"/>
-    <col min="2" max="2" width="17.8888888888889" style="30" customWidth="1"/>
-    <col min="3" max="4" width="31" style="30" customWidth="1"/>
-    <col min="5" max="5" width="20.1944444444444" style="30" customWidth="1"/>
-    <col min="6" max="16384" width="8.88888888888889" style="30"/>
+    <col min="1" max="1" width="13.4444444444444" style="29" customWidth="1"/>
+    <col min="2" max="2" width="17.8888888888889" style="29" customWidth="1"/>
+    <col min="3" max="4" width="31" style="29" customWidth="1"/>
+    <col min="5" max="5" width="20.1944444444444" style="29" customWidth="1"/>
+    <col min="6" max="16384" width="8.88888888888889" style="29"/>
   </cols>
   <sheetData>
     <row r="5" ht="15.6" spans="2:4">
-      <c r="B5" s="31" t="s">
+      <c r="B5" s="30" t="s">
         <v>31</v>
       </c>
-      <c r="C5" s="31"/>
-      <c r="D5" s="31"/>
+      <c r="C5" s="30"/>
+      <c r="D5" s="30"/>
     </row>
     <row r="6" spans="2:5">
-      <c r="B6" s="32" t="s">
+      <c r="B6" s="31" t="s">
         <v>32</v>
       </c>
-      <c r="C6" s="32" t="s">
+      <c r="C6" s="31" t="s">
         <v>33</v>
       </c>
-      <c r="D6" s="32" t="s">
+      <c r="D6" s="31" t="s">
         <v>34</v>
       </c>
-      <c r="E6" s="33"/>
+      <c r="E6" s="32"/>
     </row>
     <row r="7" ht="16" customHeight="1" spans="2:4">
-      <c r="B7" s="34" t="s">
+      <c r="B7" s="33" t="s">
         <v>35</v>
       </c>
-      <c r="C7" s="35" t="s">
+      <c r="C7" s="34" t="s">
         <v>36</v>
       </c>
-      <c r="D7" s="35" t="s">
+      <c r="D7" s="34" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="8" ht="16" customHeight="1" spans="2:4">
-      <c r="B8" s="36" t="s">
+      <c r="B8" s="35" t="s">
         <v>38</v>
       </c>
-      <c r="C8" s="35" t="s">
+      <c r="C8" s="34" t="s">
         <v>39</v>
       </c>
-      <c r="D8" s="35" t="s">
+      <c r="D8" s="34" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="9" ht="16" customHeight="1" spans="2:4">
-      <c r="B9" s="37" t="s">
+      <c r="B9" s="36" t="s">
         <v>41</v>
       </c>
-      <c r="C9" s="35" t="s">
+      <c r="C9" s="34" t="s">
         <v>42</v>
       </c>
-      <c r="D9" s="35" t="s">
+      <c r="D9" s="34" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="10" ht="16" customHeight="1" spans="2:4">
-      <c r="B10" s="38" t="s">
+      <c r="B10" s="37" t="s">
         <v>44</v>
       </c>
-      <c r="C10" s="39" t="s">
+      <c r="C10" s="38" t="s">
         <v>42</v>
       </c>
-      <c r="D10" s="39" t="s">
+      <c r="D10" s="38" t="s">
         <v>45</v>
       </c>
     </row>
@@ -2842,8 +2839,8 @@
   <sheetPr/>
   <dimension ref="C4:K11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="N3" sqref="N3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="N11" sqref="N11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="14.4"/>
@@ -2862,7 +2859,7 @@
       <c r="F5" s="3"/>
       <c r="G5" s="3"/>
       <c r="H5" s="3"/>
-      <c r="I5" s="21"/>
+      <c r="I5" s="20"/>
     </row>
     <row r="6" s="1" customFormat="1" ht="18" customHeight="1" spans="3:9">
       <c r="C6" s="4" t="s">
@@ -2906,10 +2903,10 @@
       <c r="H7" s="9">
         <v>6</v>
       </c>
-      <c r="I7" s="22">
+      <c r="I7" s="21">
         <v>7</v>
       </c>
-      <c r="K7" s="23" t="s">
+      <c r="K7" s="22" t="s">
         <v>54</v>
       </c>
     </row>
@@ -2932,10 +2929,10 @@
       <c r="H8" s="11">
         <v>13</v>
       </c>
-      <c r="I8" s="24">
+      <c r="I8" s="23">
         <v>14</v>
       </c>
-      <c r="K8" s="25" t="s">
+      <c r="K8" s="24" t="s">
         <v>55</v>
       </c>
     </row>
@@ -2955,27 +2952,27 @@
       <c r="G9" s="11">
         <v>19</v>
       </c>
-      <c r="H9" s="16">
+      <c r="H9" s="14">
         <v>20</v>
       </c>
-      <c r="I9" s="26">
+      <c r="I9" s="23">
         <v>21</v>
       </c>
-      <c r="K9" s="27" t="s">
+      <c r="K9" s="25" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="10" ht="52" customHeight="1" spans="3:11">
-      <c r="C10" s="17">
+      <c r="C10" s="10">
         <v>22</v>
       </c>
-      <c r="D10" s="16">
+      <c r="D10" s="11">
         <v>23</v>
       </c>
-      <c r="E10" s="16">
+      <c r="E10" s="11">
         <v>24</v>
       </c>
-      <c r="F10" s="16">
+      <c r="F10" s="14">
         <v>25</v>
       </c>
       <c r="G10" s="16">
@@ -2987,30 +2984,30 @@
       <c r="I10" s="26">
         <v>28</v>
       </c>
-      <c r="K10" s="28" t="s">
+      <c r="K10" s="27" t="s">
         <v>57</v>
       </c>
     </row>
     <row r="11" ht="52" customHeight="1" spans="3:9">
-      <c r="C11" s="18">
+      <c r="C11" s="17">
         <v>29</v>
       </c>
-      <c r="D11" s="19">
+      <c r="D11" s="18">
         <v>30</v>
       </c>
-      <c r="E11" s="20">
+      <c r="E11" s="19">
         <v>1</v>
       </c>
-      <c r="F11" s="20">
+      <c r="F11" s="19">
         <v>2</v>
       </c>
-      <c r="G11" s="20">
+      <c r="G11" s="19">
         <v>3</v>
       </c>
-      <c r="H11" s="20">
+      <c r="H11" s="19">
         <v>4</v>
       </c>
-      <c r="I11" s="29">
+      <c r="I11" s="28">
         <v>5</v>
       </c>
     </row>

</xml_diff>